<commit_message>
added message passing model picture#
</commit_message>
<xml_diff>
--- a/documentation/evaluation-2019-11-18.xlsx
+++ b/documentation/evaluation-2019-11-18.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="8 threads" sheetId="1" state="visible" r:id="rId1"/>
@@ -96,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="160" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -126,14 +126,30 @@
       <color indexed="2"/>
       <sz val="11"/>
     </font>
-    <font/>
     <font>
+      <name val="CMU Serif"/>
+      <color theme="1"/>
       <sz val="11"/>
     </font>
     <font>
+      <name val="CMU Serif"/>
+      <b/>
+      <color theme="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="CMU Serif"/>
+    </font>
+    <font>
+      <name val="CMU Serif"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="CMU Serif"/>
       <color theme="1" tint="0"/>
       <sz val="11"/>
     </font>
+    <font/>
   </fonts>
   <fills count="5">
     <fill/>
@@ -209,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1"/>
@@ -237,22 +253,39 @@
     <xf fontId="4" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="5" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="6" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="5" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="4" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="7" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="8" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="9" fillId="4" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="7" fillId="4" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="5" fillId="4" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="5" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="7" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="3" fillId="0" borderId="4" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="10" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="10" fillId="4" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="10" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="3" fillId="4" borderId="4" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1532,10 +1565,18 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US">
+                <a:latin typeface="CMU Serif"/>
+                <a:ea typeface="CMU Serif"/>
+                <a:cs typeface="CMU Serif"/>
+              </a:rPr>
               <a:t>Total speedup in dependence of </a:t>
             </a:r>
-            <a:endParaRPr/>
+            <a:endParaRPr>
+              <a:latin typeface="CMU Serif"/>
+              <a:ea typeface="CMU Serif"/>
+              <a:cs typeface="CMU Serif"/>
+            </a:endParaRPr>
           </a:p>
           <a:p>
             <a:pPr>
@@ -1549,10 +1590,18 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US">
+                <a:latin typeface="CMU Serif"/>
+                <a:ea typeface="CMU Serif"/>
+                <a:cs typeface="CMU Serif"/>
+              </a:rPr>
               <a:t>used amount of threads</a:t>
             </a:r>
-            <a:endParaRPr/>
+            <a:endParaRPr>
+              <a:latin typeface="CMU Serif"/>
+              <a:ea typeface="CMU Serif"/>
+              <a:cs typeface="CMU Serif"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1848,6 +1897,7 @@
         <c:dLbls>
           <c:showBubbleSize val="0"/>
           <c:showCatName val="0"/>
+          <c:showLeaderLines val="0"/>
           <c:showLegendKey val="0"/>
           <c:showPercent val="0"/>
           <c:showSerName val="0"/>
@@ -1874,10 +1924,18 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr/>
+                  <a:rPr>
+                    <a:latin typeface="CMU Serif"/>
+                    <a:ea typeface="CMU Serif"/>
+                    <a:cs typeface="CMU Serif"/>
+                  </a:rPr>
                   <a:t>number of threads</a:t>
                 </a:r>
-                <a:endParaRPr/>
+                <a:endParaRPr>
+                  <a:latin typeface="CMU Serif"/>
+                  <a:ea typeface="CMU Serif"/>
+                  <a:cs typeface="CMU Serif"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1922,6 +1980,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:latin typeface="CMU Serif"/>
+                <a:ea typeface="CMU Serif"/>
+                <a:cs typeface="CMU Serif"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr/>
@@ -1969,22 +2030,42 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr/>
-                  <a:t>SPeedup S = T</a:t>
+                  <a:rPr>
+                    <a:latin typeface="CMU Serif"/>
+                    <a:ea typeface="CMU Serif"/>
+                    <a:cs typeface="CMU Serif"/>
+                  </a:rPr>
+                  <a:t>Speedup S = T</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr baseline="-25000"/>
+                  <a:rPr baseline="-25000">
+                    <a:latin typeface="CMU Serif"/>
+                    <a:ea typeface="CMU Serif"/>
+                    <a:cs typeface="CMU Serif"/>
+                  </a:rPr>
                   <a:t>1</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr/>
+                  <a:rPr>
+                    <a:latin typeface="CMU Serif"/>
+                    <a:ea typeface="CMU Serif"/>
+                    <a:cs typeface="CMU Serif"/>
+                  </a:rPr>
                   <a:t> / T</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr baseline="-25000"/>
+                  <a:rPr baseline="-25000">
+                    <a:latin typeface="CMU Serif"/>
+                    <a:ea typeface="CMU Serif"/>
+                    <a:cs typeface="CMU Serif"/>
+                  </a:rPr>
                   <a:t>P</a:t>
                 </a:r>
-                <a:endParaRPr/>
+                <a:endParaRPr>
+                  <a:latin typeface="CMU Serif"/>
+                  <a:ea typeface="CMU Serif"/>
+                  <a:cs typeface="CMU Serif"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2024,6 +2105,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:latin typeface="CMU Serif"/>
+                <a:ea typeface="CMU Serif"/>
+                <a:cs typeface="CMU Serif"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr/>
@@ -2047,6 +2131,19 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="CMU Serif"/>
+              <a:ea typeface="CMU Serif"/>
+              <a:cs typeface="CMU Serif"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -2054,7 +2151,7 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm>
-      <a:off x="8762999" y="182540"/>
+      <a:off x="9182098" y="182539"/>
       <a:ext cx="7858123" cy="5294333"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
@@ -2628,6 +2725,7 @@
         <c:dLbls>
           <c:showBubbleSize val="0"/>
           <c:showCatName val="0"/>
+          <c:showLeaderLines val="0"/>
           <c:showLegendKey val="0"/>
           <c:showPercent val="0"/>
           <c:showSerName val="0"/>
@@ -3181,6 +3279,14 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showBubbleSize val="0"/>
+          <c:showCatName val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showPercent val="0"/>
+          <c:showSerName val="0"/>
+          <c:showVal val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1025"/>
@@ -3256,6 +3362,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1026"/>
+        <c:crosses val="autoZero"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3527,16 +3634,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600073</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1565</xdr:rowOff>
+      <xdr:rowOff>1564</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>552448</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>533396</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76197</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3546,7 +3653,7 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8762999" y="182540"/>
+        <a:off x="9182098" y="182539"/>
         <a:ext cx="7858123" cy="5294333"/>
       </xdr:xfrm>
       <a:graphic>
@@ -4859,633 +4966,634 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.421875"/>
-    <col customWidth="1" min="2" max="2" width="22.7109375"/>
-    <col customWidth="1" min="3" max="4" width="18.421875"/>
-    <col customWidth="1" min="5" max="6" width="25.00390625"/>
+    <col customWidth="1" min="1" max="1" style="11" width="3.421875"/>
+    <col customWidth="1" min="2" max="2" style="11" width="22.7109375"/>
+    <col customWidth="1" min="3" max="4" style="11" width="22.00390625"/>
+    <col customWidth="1" min="5" max="6" style="11" width="29.28125"/>
+    <col min="7" max="16384" style="11" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="2" ht="16.5">
-      <c r="B2" s="6" t="s">
+    <row r="2" ht="17.25">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
-      <c r="B3" s="7">
+    <row r="3" ht="15.75">
+      <c r="B3" s="13">
         <v>1</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="14">
         <v>1</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="14">
         <v>1</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="13">
         <v>41980</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="15">
         <v>41980</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" s="7">
+    <row r="4" ht="15.75">
+      <c r="B4" s="13">
         <v>2</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="14">
         <f t="shared" ref="C4:C9" si="2">$E$3/E4</f>
         <v>1.5994818258020269</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="14">
         <f t="shared" ref="D4:D9" si="3">$F$3/F4</f>
         <v>1.5994818258020269</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="13">
         <v>26246</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="15">
         <v>26246</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" s="7">
+    <row r="5" ht="15.75">
+      <c r="B5" s="13">
         <v>3</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="14">
         <f t="shared" si="2"/>
         <v>2.0002858912660217</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="14">
         <f t="shared" si="3"/>
         <v>2.0001905850962456</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="16">
         <v>20987</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="15">
         <v>20988</v>
       </c>
     </row>
-    <row r="6">
-      <c r="B6" s="7">
+    <row r="6" ht="15.75">
+      <c r="B6" s="13">
         <v>4</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="14">
         <f t="shared" si="2"/>
         <v>2.1808925138968256</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="14">
         <f t="shared" si="3"/>
         <v>2.1808925138968256</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="16">
         <v>19249</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="15">
         <v>19249</v>
       </c>
     </row>
-    <row r="7">
-      <c r="B7" s="7">
+    <row r="7" ht="15.75">
+      <c r="B7" s="13">
         <v>5</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="14">
         <f t="shared" si="2"/>
         <v>2.4989582713256739</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="14">
         <f t="shared" si="3"/>
         <v>2.4989582713256739</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="16">
         <v>16799</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="15">
         <v>16799</v>
       </c>
     </row>
-    <row r="8">
-      <c r="B8" s="7">
+    <row r="8" ht="15.75">
+      <c r="B8" s="13">
         <v>6</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="14">
         <f t="shared" si="2"/>
         <v>2.5242017918345261</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="14">
         <f t="shared" si="3"/>
         <v>2.5242017918345261</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="16">
         <v>16631</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="15">
         <v>16631</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" s="7">
+    <row r="9" ht="15.75">
+      <c r="B9" s="13">
         <v>7</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="14">
         <f t="shared" si="2"/>
         <v>2.7962432558449346</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="14">
         <f t="shared" si="3"/>
         <v>2.7962432558449346</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="16">
         <v>15013</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="15">
         <v>15013</v>
       </c>
     </row>
-    <row r="10">
-      <c r="B10" s="7">
+    <row r="10" ht="15.75">
+      <c r="B10" s="13">
         <v>8</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="14">
         <f t="shared" ref="C10:C34" si="4">$E$3/E10</f>
         <v>2.7544124401286005</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="14">
         <f t="shared" ref="D10:D34" si="5">$F$3/F10</f>
         <v>2.7544124401286005</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="16">
         <v>15241</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="15">
         <v>15241</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" s="7">
+    <row r="11" ht="15.75">
+      <c r="B11" s="13">
         <v>9</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="14">
         <f t="shared" si="4"/>
         <v>2.9938667807730708</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="14">
         <f t="shared" si="5"/>
         <v>2.9938667807730708</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="16">
         <v>14022</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="15">
         <v>14022</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="7">
+    <row r="12" ht="15.75">
+      <c r="B12" s="13">
         <v>10</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="14">
         <f t="shared" si="4"/>
         <v>2.9203478260869566</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="14">
         <f t="shared" si="5"/>
         <v>2.9205509948518156</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="16">
         <v>14375</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="15">
         <v>14374</v>
       </c>
     </row>
-    <row r="13">
-      <c r="B13" s="7">
+    <row r="13" ht="15.75">
+      <c r="B13" s="13">
         <v>11</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="14">
         <f t="shared" si="4"/>
         <v>3.1335373591102487</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="14">
         <f t="shared" si="5"/>
         <v>3.1335373591102487</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="16">
         <v>13397</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="15">
         <v>13397</v>
       </c>
     </row>
-    <row r="14">
-      <c r="B14" s="7">
+    <row r="14" ht="15.75">
+      <c r="B14" s="13">
         <v>12</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="14">
         <f t="shared" si="4"/>
         <v>3.0448973670849351</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="14">
         <f t="shared" si="5"/>
         <v>3.0448973670849351</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="16">
         <v>13787</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="15">
         <v>13787</v>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" s="7">
+    <row r="15" ht="15.75">
+      <c r="B15" s="13">
         <v>13</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="14">
         <f t="shared" si="4"/>
         <v>3.23769859632886</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="14">
         <f t="shared" si="5"/>
         <v>3.23769859632886</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="16">
         <v>12966</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="15">
         <v>12966</v>
       </c>
     </row>
-    <row r="16">
-      <c r="B16" s="7">
+    <row r="16" ht="15.75">
+      <c r="B16" s="13">
         <v>14</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="14">
         <f t="shared" si="4"/>
         <v>3.1419803906893198</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="14">
         <f t="shared" si="5"/>
         <v>3.1419803906893198</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="16">
         <v>13361</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="15">
         <v>13361</v>
       </c>
     </row>
-    <row r="17">
-      <c r="B17" s="7">
+    <row r="17" ht="15.75">
+      <c r="B17" s="13">
         <v>15</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="14">
         <f t="shared" si="4"/>
         <v>3.3172659028052154</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="14">
         <f t="shared" si="5"/>
         <v>3.3172659028052154</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="16">
         <v>12655</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="15">
         <v>12655</v>
       </c>
     </row>
-    <row r="18">
-      <c r="B18" s="7">
+    <row r="18" ht="15.75">
+      <c r="B18" s="13">
         <v>16</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="14">
         <f t="shared" si="4"/>
         <v>3.2198189906427368</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="14">
         <f t="shared" si="5"/>
         <v>3.2198189906427368</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="16">
         <v>13038</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="15">
         <v>13038</v>
       </c>
     </row>
-    <row r="19">
-      <c r="B19" s="7">
+    <row r="19" ht="15.75">
+      <c r="B19" s="13">
         <v>17</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="14">
         <f t="shared" si="4"/>
         <v>3.3794880051521492</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="14">
         <f t="shared" si="5"/>
         <v>3.3794880051521492</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="16">
         <v>12422</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="15">
         <v>12422</v>
       </c>
     </row>
-    <row r="20">
-      <c r="B20" s="7">
+    <row r="20" ht="15.75">
+      <c r="B20" s="13">
         <v>18</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="14">
         <f t="shared" si="4"/>
         <v>3.2853341681014245</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="14">
         <f t="shared" si="5"/>
         <v>3.2853341681014245</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="16">
         <v>12778</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="15">
         <v>12778</v>
       </c>
     </row>
-    <row r="21">
-      <c r="B21" s="7">
+    <row r="21" ht="15.75">
+      <c r="B21" s="13">
         <v>19</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="14">
         <f t="shared" si="4"/>
         <v>3.4288981458792778</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="14">
         <f t="shared" si="5"/>
         <v>3.4288981458792778</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="16">
         <v>12243</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="15">
         <v>12243</v>
       </c>
     </row>
-    <row r="22">
-      <c r="B22" s="7">
+    <row r="22" ht="15.75">
+      <c r="B22" s="13">
         <v>20</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="14">
         <f t="shared" si="4"/>
         <v>3.3346572404480104</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="14">
         <f t="shared" si="5"/>
         <v>3.3346572404480104</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="16">
         <v>12589</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="15">
         <v>12589</v>
       </c>
     </row>
-    <row r="23">
-      <c r="B23" s="7">
+    <row r="23" ht="15.75">
+      <c r="B23" s="13">
         <v>21</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="14">
         <f t="shared" si="4"/>
         <v>3.4708557255064076</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="14">
         <f t="shared" si="5"/>
         <v>3.4705687830687832</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="16">
         <v>12095</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="15">
         <v>12096</v>
       </c>
     </row>
-    <row r="24">
-      <c r="B24" s="7">
+    <row r="24" ht="15.75">
+      <c r="B24" s="13">
         <v>22</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="14">
         <f t="shared" si="4"/>
         <v>3.3797600837291681</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="14">
         <f t="shared" si="5"/>
         <v>3.3797600837291681</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="16">
         <v>12421</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="15">
         <v>12421</v>
       </c>
     </row>
-    <row r="25">
-      <c r="B25" s="7">
+    <row r="25" ht="15.75">
+      <c r="B25" s="13">
         <v>23</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="14">
         <f t="shared" si="4"/>
         <v>3.5050513484178007</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="14">
         <f t="shared" si="5"/>
         <v>3.5050513484178007</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="16">
         <v>11977</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="15">
         <v>11977</v>
       </c>
     </row>
-    <row r="26">
-      <c r="B26" s="7">
+    <row r="26" ht="15.75">
+      <c r="B26" s="13">
         <v>24</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="14">
         <f t="shared" si="4"/>
         <v>3.4168972814585707</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="14">
         <f t="shared" si="5"/>
         <v>3.4160631459028399</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="16">
         <v>12286</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="15">
         <v>12289</v>
       </c>
     </row>
-    <row r="27">
-      <c r="B27" s="7">
+    <row r="27" ht="15.75">
+      <c r="B27" s="13">
         <v>25</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="14">
         <f t="shared" si="4"/>
         <v>3.5345625999831607</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="14">
         <f t="shared" si="5"/>
         <v>3.5345625999831607</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="16">
         <v>11877</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="15">
         <v>11877</v>
       </c>
     </row>
-    <row r="28">
-      <c r="B28" s="7">
+    <row r="28" ht="15.75">
+      <c r="B28" s="13">
         <v>26</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="14">
         <f t="shared" si="4"/>
         <v>3.4469168240413826</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="14">
         <f t="shared" si="5"/>
         <v>3.4469168240413826</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="17">
         <v>12179</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="18">
         <v>12179</v>
       </c>
     </row>
-    <row r="29">
-      <c r="B29" s="7">
+    <row r="29" ht="15.75">
+      <c r="B29" s="13">
         <v>27</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="14">
         <f t="shared" si="4"/>
         <v>3.5558190750465863</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="14">
         <f t="shared" si="5"/>
         <v>3.5558190750465863</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="17">
         <v>11806</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="18">
         <v>11806</v>
       </c>
     </row>
-    <row r="30">
-      <c r="B30" s="7">
+    <row r="30" ht="15.75">
+      <c r="B30" s="13">
         <v>28</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="14">
         <f t="shared" si="4"/>
         <v>3.476316661146075</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="14">
         <f t="shared" si="5"/>
         <v>3.4760288151030885</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="17">
         <v>12076</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="18">
         <v>12077</v>
       </c>
     </row>
-    <row r="31">
-      <c r="B31" s="7">
+    <row r="31" ht="15.75">
+      <c r="B31" s="13">
         <v>29</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="14">
         <f t="shared" si="4"/>
         <v>3.5800784581272387</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="14">
         <f t="shared" si="5"/>
         <v>3.5800784581272387</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="17">
         <v>11726</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="18">
         <v>11726</v>
       </c>
     </row>
-    <row r="32">
-      <c r="B32" s="7">
+    <row r="32" ht="15.75">
+      <c r="B32" s="13">
         <v>30</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="14">
         <f t="shared" si="4"/>
         <v>3.5006671114076049</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="14">
         <f t="shared" si="5"/>
         <v>3.501835168501835</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="17">
         <v>11992</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="18">
         <v>11988</v>
       </c>
     </row>
-    <row r="33">
-      <c r="B33" s="7">
+    <row r="33" ht="15.75">
+      <c r="B33" s="13">
         <v>31</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="14">
         <f t="shared" si="4"/>
         <v>3.5947936290460696</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="14">
         <f t="shared" si="5"/>
         <v>3.5960253554908341</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="17">
         <v>11678</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="18">
         <v>11674</v>
       </c>
-      <c r="K33" s="15"/>
-    </row>
-    <row r="34">
-      <c r="B34" s="7">
+      <c r="K33" s="19"/>
+    </row>
+    <row r="34" ht="15.75">
+      <c r="B34" s="13">
         <v>32</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="14">
         <f t="shared" si="4"/>
         <v>3.5218120805369129</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="14">
         <f t="shared" si="5"/>
         <v>3.5221075593590068</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="17">
         <v>11920</v>
       </c>
-      <c r="F34" s="14">
+      <c r="F34" s="18">
         <v>11919</v>
       </c>
     </row>
@@ -5538,20 +5646,20 @@
       <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="20">
         <v>1</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="20">
         <v>1</v>
       </c>
-      <c r="E3" s="16">
-        <f>ABS(C3-D3)</f>
+      <c r="E3" s="20">
+        <f t="shared" ref="E3:E9" si="6">ABS(C3-D3)</f>
         <v>0</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="21">
         <v>41980</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="21">
         <v>41980</v>
       </c>
     </row>
@@ -5559,22 +5667,22 @@
       <c r="B4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="16">
-        <f t="shared" ref="C4:C9" si="6">$F$3/F4</f>
+      <c r="C4" s="20">
+        <f t="shared" ref="C4:C9" si="7">$F$3/F4</f>
         <v>1.5994818258020269</v>
       </c>
-      <c r="D4" s="16">
-        <f t="shared" ref="D4:D9" si="7">$G$3/G4</f>
+      <c r="D4" s="20">
+        <f t="shared" ref="D4:D9" si="8">$G$3/G4</f>
         <v>1.5994818258020269</v>
       </c>
-      <c r="E4" s="16">
-        <f>ABS(C4-D4)</f>
+      <c r="E4" s="20">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="21">
         <v>26246</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="21">
         <v>26246</v>
       </c>
     </row>
@@ -5582,22 +5690,22 @@
       <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="16">
-        <f t="shared" si="6"/>
-        <v>2.0001905850962456</v>
-      </c>
-      <c r="D5" s="16">
+      <c r="C5" s="20">
         <f t="shared" si="7"/>
         <v>2.0001905850962456</v>
       </c>
-      <c r="E5" s="16">
-        <f>ABS(C5-D5)</f>
+      <c r="D5" s="20">
+        <f t="shared" si="8"/>
+        <v>2.0001905850962456</v>
+      </c>
+      <c r="E5" s="20">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="21">
         <v>20988</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="21">
         <v>20988</v>
       </c>
     </row>
@@ -5605,22 +5713,22 @@
       <c r="B6" s="7">
         <v>4</v>
       </c>
-      <c r="C6" s="16">
-        <f t="shared" si="6"/>
-        <v>2.1808925138968256</v>
-      </c>
-      <c r="D6" s="16">
+      <c r="C6" s="20">
         <f t="shared" si="7"/>
         <v>2.1808925138968256</v>
       </c>
-      <c r="E6" s="16">
-        <f>ABS(C6-D6)</f>
+      <c r="D6" s="20">
+        <f t="shared" si="8"/>
+        <v>2.1808925138968256</v>
+      </c>
+      <c r="E6" s="20">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="21">
         <v>19249</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="21">
         <v>19249</v>
       </c>
     </row>
@@ -5628,22 +5736,22 @@
       <c r="B7" s="7">
         <v>5</v>
       </c>
-      <c r="C7" s="16">
-        <f t="shared" si="6"/>
-        <v>2.4989582713256739</v>
-      </c>
-      <c r="D7" s="16">
+      <c r="C7" s="20">
         <f t="shared" si="7"/>
         <v>2.4989582713256739</v>
       </c>
-      <c r="E7" s="16">
-        <f>ABS(C7-D7)</f>
+      <c r="D7" s="20">
+        <f t="shared" si="8"/>
+        <v>2.4989582713256739</v>
+      </c>
+      <c r="E7" s="20">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="21">
         <v>16799</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="21">
         <v>16799</v>
       </c>
     </row>
@@ -5651,22 +5759,22 @@
       <c r="B8" s="7">
         <v>6</v>
       </c>
-      <c r="C8" s="16">
-        <f t="shared" si="6"/>
-        <v>2.5242017918345261</v>
-      </c>
-      <c r="D8" s="16">
+      <c r="C8" s="20">
         <f t="shared" si="7"/>
         <v>2.5242017918345261</v>
       </c>
-      <c r="E8" s="16">
-        <f>ABS(C8-D8)</f>
+      <c r="D8" s="20">
+        <f t="shared" si="8"/>
+        <v>2.5242017918345261</v>
+      </c>
+      <c r="E8" s="20">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="21">
         <v>16631</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="21">
         <v>16631</v>
       </c>
     </row>
@@ -5674,22 +5782,22 @@
       <c r="B9" s="7">
         <v>7</v>
       </c>
-      <c r="C9" s="16">
-        <f t="shared" si="6"/>
-        <v>2.7962432558449346</v>
-      </c>
-      <c r="D9" s="16">
+      <c r="C9" s="20">
         <f t="shared" si="7"/>
         <v>2.7962432558449346</v>
       </c>
-      <c r="E9" s="16">
-        <f>ABS(C9-D9)</f>
+      <c r="D9" s="20">
+        <f t="shared" si="8"/>
+        <v>2.7962432558449346</v>
+      </c>
+      <c r="E9" s="20">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="21">
         <v>15013</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="21">
         <v>15013</v>
       </c>
     </row>
@@ -5697,22 +5805,22 @@
       <c r="B10" s="7">
         <v>8</v>
       </c>
-      <c r="C10" s="16">
-        <f t="shared" ref="C10:C66" si="8">$F$3/F10</f>
+      <c r="C10" s="20">
+        <f t="shared" ref="C10:C66" si="9">$F$3/F10</f>
         <v>2.7544124401286005</v>
       </c>
-      <c r="D10" s="16">
-        <f t="shared" ref="D10:D66" si="9">$G$3/G10</f>
+      <c r="D10" s="20">
+        <f t="shared" ref="D10:D66" si="10">$G$3/G10</f>
         <v>2.7544124401286005</v>
       </c>
-      <c r="E10" s="16">
-        <f>ABS(C10-D10)</f>
+      <c r="E10" s="20">
+        <f t="shared" ref="E10:E66" si="11">ABS(C10-D10)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="21">
         <v>15241</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="21">
         <v>15241</v>
       </c>
     </row>
@@ -5720,22 +5828,22 @@
       <c r="B11" s="7">
         <v>9</v>
       </c>
-      <c r="C11" s="16">
-        <f t="shared" si="8"/>
-        <v>2.9938667807730708</v>
-      </c>
-      <c r="D11" s="16">
+      <c r="C11" s="20">
         <f t="shared" si="9"/>
         <v>2.9938667807730708</v>
       </c>
-      <c r="E11" s="16">
-        <f>ABS(C11-D11)</f>
+      <c r="D11" s="20">
+        <f t="shared" si="10"/>
+        <v>2.9938667807730708</v>
+      </c>
+      <c r="E11" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="21">
         <v>14022</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="21">
         <v>14022</v>
       </c>
     </row>
@@ -5743,22 +5851,22 @@
       <c r="B12" s="7">
         <v>10</v>
       </c>
-      <c r="C12" s="16">
-        <f t="shared" si="8"/>
-        <v>2.9205509948518156</v>
-      </c>
-      <c r="D12" s="16">
+      <c r="C12" s="20">
         <f t="shared" si="9"/>
         <v>2.9205509948518156</v>
       </c>
-      <c r="E12" s="16">
-        <f>ABS(C12-D12)</f>
+      <c r="D12" s="20">
+        <f t="shared" si="10"/>
+        <v>2.9205509948518156</v>
+      </c>
+      <c r="E12" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="21">
         <v>14374</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="21">
         <v>14374</v>
       </c>
     </row>
@@ -5766,22 +5874,22 @@
       <c r="B13" s="7">
         <v>11</v>
       </c>
-      <c r="C13" s="16">
-        <f t="shared" si="8"/>
-        <v>3.1335373591102487</v>
-      </c>
-      <c r="D13" s="16">
+      <c r="C13" s="20">
         <f t="shared" si="9"/>
         <v>3.1335373591102487</v>
       </c>
-      <c r="E13" s="16">
-        <f>ABS(C13-D13)</f>
+      <c r="D13" s="20">
+        <f t="shared" si="10"/>
+        <v>3.1335373591102487</v>
+      </c>
+      <c r="E13" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="21">
         <v>13397</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="21">
         <v>13397</v>
       </c>
     </row>
@@ -5789,22 +5897,22 @@
       <c r="B14" s="7">
         <v>12</v>
       </c>
-      <c r="C14" s="16">
-        <f t="shared" si="8"/>
-        <v>3.0448973670849351</v>
-      </c>
-      <c r="D14" s="16">
+      <c r="C14" s="20">
         <f t="shared" si="9"/>
         <v>3.0448973670849351</v>
       </c>
-      <c r="E14" s="16">
-        <f>ABS(C14-D14)</f>
+      <c r="D14" s="20">
+        <f t="shared" si="10"/>
+        <v>3.0448973670849351</v>
+      </c>
+      <c r="E14" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="21">
         <v>13787</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="21">
         <v>13787</v>
       </c>
     </row>
@@ -5812,22 +5920,22 @@
       <c r="B15" s="7">
         <v>13</v>
       </c>
-      <c r="C15" s="16">
-        <f t="shared" si="8"/>
-        <v>3.23769859632886</v>
-      </c>
-      <c r="D15" s="16">
+      <c r="C15" s="20">
         <f t="shared" si="9"/>
         <v>3.23769859632886</v>
       </c>
-      <c r="E15" s="16">
-        <f>ABS(C15-D15)</f>
+      <c r="D15" s="20">
+        <f t="shared" si="10"/>
+        <v>3.23769859632886</v>
+      </c>
+      <c r="E15" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="21">
         <v>12966</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="21">
         <v>12966</v>
       </c>
     </row>
@@ -5835,22 +5943,22 @@
       <c r="B16" s="7">
         <v>14</v>
       </c>
-      <c r="C16" s="16">
-        <f t="shared" si="8"/>
-        <v>3.1419803906893198</v>
-      </c>
-      <c r="D16" s="16">
+      <c r="C16" s="20">
         <f t="shared" si="9"/>
         <v>3.1419803906893198</v>
       </c>
-      <c r="E16" s="16">
-        <f>ABS(C16-D16)</f>
+      <c r="D16" s="20">
+        <f t="shared" si="10"/>
+        <v>3.1419803906893198</v>
+      </c>
+      <c r="E16" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="21">
         <v>13361</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="21">
         <v>13361</v>
       </c>
     </row>
@@ -5858,22 +5966,22 @@
       <c r="B17" s="7">
         <v>15</v>
       </c>
-      <c r="C17" s="16">
-        <f t="shared" si="8"/>
-        <v>3.3172659028052154</v>
-      </c>
-      <c r="D17" s="16">
+      <c r="C17" s="20">
         <f t="shared" si="9"/>
         <v>3.3172659028052154</v>
       </c>
-      <c r="E17" s="16">
-        <f>ABS(C17-D17)</f>
+      <c r="D17" s="20">
+        <f t="shared" si="10"/>
+        <v>3.3172659028052154</v>
+      </c>
+      <c r="E17" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="21">
         <v>12655</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="21">
         <v>12655</v>
       </c>
     </row>
@@ -5881,22 +5989,22 @@
       <c r="B18" s="7">
         <v>16</v>
       </c>
-      <c r="C18" s="16">
-        <f t="shared" si="8"/>
-        <v>3.2198189906427368</v>
-      </c>
-      <c r="D18" s="16">
+      <c r="C18" s="20">
         <f t="shared" si="9"/>
         <v>3.2198189906427368</v>
       </c>
-      <c r="E18" s="16">
-        <f>ABS(C18-D18)</f>
+      <c r="D18" s="20">
+        <f t="shared" si="10"/>
+        <v>3.2198189906427368</v>
+      </c>
+      <c r="E18" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="21">
         <v>13038</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="21">
         <v>13038</v>
       </c>
     </row>
@@ -5904,22 +6012,22 @@
       <c r="B19" s="7">
         <v>17</v>
       </c>
-      <c r="C19" s="16">
-        <f t="shared" si="8"/>
-        <v>3.3794880051521492</v>
-      </c>
-      <c r="D19" s="16">
+      <c r="C19" s="20">
         <f t="shared" si="9"/>
         <v>3.3794880051521492</v>
       </c>
-      <c r="E19" s="16">
-        <f>ABS(C19-D19)</f>
+      <c r="D19" s="20">
+        <f t="shared" si="10"/>
+        <v>3.3794880051521492</v>
+      </c>
+      <c r="E19" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="21">
         <v>12422</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="21">
         <v>12422</v>
       </c>
     </row>
@@ -5927,22 +6035,22 @@
       <c r="B20" s="7">
         <v>18</v>
       </c>
-      <c r="C20" s="16">
-        <f t="shared" si="8"/>
-        <v>3.2853341681014245</v>
-      </c>
-      <c r="D20" s="16">
+      <c r="C20" s="20">
         <f t="shared" si="9"/>
         <v>3.2853341681014245</v>
       </c>
-      <c r="E20" s="16">
-        <f>ABS(C20-D20)</f>
+      <c r="D20" s="20">
+        <f t="shared" si="10"/>
+        <v>3.2853341681014245</v>
+      </c>
+      <c r="E20" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="21">
         <v>12778</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="21">
         <v>12778</v>
       </c>
     </row>
@@ -5950,22 +6058,22 @@
       <c r="B21" s="7">
         <v>19</v>
       </c>
-      <c r="C21" s="16">
-        <f t="shared" si="8"/>
-        <v>3.4288981458792778</v>
-      </c>
-      <c r="D21" s="16">
+      <c r="C21" s="20">
         <f t="shared" si="9"/>
         <v>3.4288981458792778</v>
       </c>
-      <c r="E21" s="16">
-        <f>ABS(C21-D21)</f>
+      <c r="D21" s="20">
+        <f t="shared" si="10"/>
+        <v>3.4288981458792778</v>
+      </c>
+      <c r="E21" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="21">
         <v>12243</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="21">
         <v>12243</v>
       </c>
     </row>
@@ -5973,22 +6081,22 @@
       <c r="B22" s="7">
         <v>20</v>
       </c>
-      <c r="C22" s="16">
-        <f t="shared" si="8"/>
-        <v>3.3346572404480104</v>
-      </c>
-      <c r="D22" s="16">
+      <c r="C22" s="20">
         <f t="shared" si="9"/>
         <v>3.3346572404480104</v>
       </c>
-      <c r="E22" s="16">
-        <f>ABS(C22-D22)</f>
+      <c r="D22" s="20">
+        <f t="shared" si="10"/>
+        <v>3.3346572404480104</v>
+      </c>
+      <c r="E22" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="21">
         <v>12589</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="21">
         <v>12589</v>
       </c>
     </row>
@@ -5996,22 +6104,22 @@
       <c r="B23" s="7">
         <v>21</v>
       </c>
-      <c r="C23" s="16">
-        <f t="shared" si="8"/>
-        <v>3.4705687830687832</v>
-      </c>
-      <c r="D23" s="16">
+      <c r="C23" s="20">
         <f t="shared" si="9"/>
         <v>3.4705687830687832</v>
       </c>
-      <c r="E23" s="16">
-        <f>ABS(C23-D23)</f>
+      <c r="D23" s="20">
+        <f t="shared" si="10"/>
+        <v>3.4705687830687832</v>
+      </c>
+      <c r="E23" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="21">
         <v>12096</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="21">
         <v>12096</v>
       </c>
     </row>
@@ -6019,22 +6127,22 @@
       <c r="B24" s="7">
         <v>22</v>
       </c>
-      <c r="C24" s="16">
-        <f t="shared" si="8"/>
-        <v>3.3797600837291681</v>
-      </c>
-      <c r="D24" s="16">
+      <c r="C24" s="20">
         <f t="shared" si="9"/>
         <v>3.3797600837291681</v>
       </c>
-      <c r="E24" s="16">
-        <f>ABS(C24-D24)</f>
+      <c r="D24" s="20">
+        <f t="shared" si="10"/>
+        <v>3.3797600837291681</v>
+      </c>
+      <c r="E24" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="21">
         <v>12421</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="21">
         <v>12421</v>
       </c>
     </row>
@@ -6042,22 +6150,22 @@
       <c r="B25" s="7">
         <v>23</v>
       </c>
-      <c r="C25" s="16">
-        <f t="shared" si="8"/>
-        <v>3.5050513484178007</v>
-      </c>
-      <c r="D25" s="16">
+      <c r="C25" s="20">
         <f t="shared" si="9"/>
         <v>3.5050513484178007</v>
       </c>
-      <c r="E25" s="16">
-        <f>ABS(C25-D25)</f>
+      <c r="D25" s="20">
+        <f t="shared" si="10"/>
+        <v>3.5050513484178007</v>
+      </c>
+      <c r="E25" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="21">
         <v>11977</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="21">
         <v>11977</v>
       </c>
     </row>
@@ -6065,22 +6173,22 @@
       <c r="B26" s="7">
         <v>24</v>
       </c>
-      <c r="C26" s="16">
-        <f t="shared" si="8"/>
-        <v>3.4168972814585707</v>
-      </c>
-      <c r="D26" s="16">
+      <c r="C26" s="20">
         <f t="shared" si="9"/>
         <v>3.4168972814585707</v>
       </c>
-      <c r="E26" s="16">
-        <f>ABS(C26-D26)</f>
+      <c r="D26" s="20">
+        <f t="shared" si="10"/>
+        <v>3.4168972814585707</v>
+      </c>
+      <c r="E26" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="21">
         <v>12286</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="21">
         <v>12286</v>
       </c>
     </row>
@@ -6088,22 +6196,22 @@
       <c r="B27" s="7">
         <v>25</v>
       </c>
-      <c r="C27" s="16">
-        <f t="shared" si="8"/>
-        <v>3.5345625999831607</v>
-      </c>
-      <c r="D27" s="16">
+      <c r="C27" s="20">
         <f t="shared" si="9"/>
         <v>3.5345625999831607</v>
       </c>
-      <c r="E27" s="16">
-        <f>ABS(C27-D27)</f>
+      <c r="D27" s="20">
+        <f t="shared" si="10"/>
+        <v>3.5345625999831607</v>
+      </c>
+      <c r="E27" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="21">
         <v>11877</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="21">
         <v>11877</v>
       </c>
     </row>
@@ -6111,22 +6219,22 @@
       <c r="B28" s="7">
         <v>26</v>
       </c>
-      <c r="C28" s="16">
-        <f t="shared" si="8"/>
-        <v>3.4469168240413826</v>
-      </c>
-      <c r="D28" s="16">
+      <c r="C28" s="20">
         <f t="shared" si="9"/>
         <v>3.4469168240413826</v>
       </c>
-      <c r="E28" s="16">
-        <f>ABS(C28-D28)</f>
+      <c r="D28" s="20">
+        <f t="shared" si="10"/>
+        <v>3.4469168240413826</v>
+      </c>
+      <c r="E28" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="22">
         <v>12179</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="22">
         <v>12179</v>
       </c>
     </row>
@@ -6134,22 +6242,22 @@
       <c r="B29" s="7">
         <v>27</v>
       </c>
-      <c r="C29" s="16">
-        <f t="shared" si="8"/>
-        <v>3.5558190750465863</v>
-      </c>
-      <c r="D29" s="16">
+      <c r="C29" s="20">
         <f t="shared" si="9"/>
         <v>3.5558190750465863</v>
       </c>
-      <c r="E29" s="16">
-        <f>ABS(C29-D29)</f>
+      <c r="D29" s="20">
+        <f t="shared" si="10"/>
+        <v>3.5558190750465863</v>
+      </c>
+      <c r="E29" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="22">
         <v>11806</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="22">
         <v>11806</v>
       </c>
     </row>
@@ -6157,22 +6265,22 @@
       <c r="B30" s="7">
         <v>28</v>
       </c>
-      <c r="C30" s="16">
-        <f t="shared" si="8"/>
+      <c r="C30" s="20">
+        <f t="shared" si="9"/>
         <v>3.4760288151030885</v>
       </c>
-      <c r="D30" s="16">
-        <f t="shared" si="9"/>
+      <c r="D30" s="20">
+        <f t="shared" si="10"/>
         <v>3.476316661146075</v>
       </c>
-      <c r="E30" s="16">
-        <f>ABS(C30-D30)</f>
+      <c r="E30" s="20">
+        <f t="shared" si="11"/>
         <v>0.00028784604298648375</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="22">
         <v>12077</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="22">
         <v>12076</v>
       </c>
     </row>
@@ -6180,22 +6288,22 @@
       <c r="B31" s="7">
         <v>29</v>
       </c>
-      <c r="C31" s="16">
-        <f t="shared" si="8"/>
-        <v>3.5800784581272387</v>
-      </c>
-      <c r="D31" s="16">
+      <c r="C31" s="20">
         <f t="shared" si="9"/>
         <v>3.5800784581272387</v>
       </c>
-      <c r="E31" s="16">
-        <f>ABS(C31-D31)</f>
+      <c r="D31" s="20">
+        <f t="shared" si="10"/>
+        <v>3.5800784581272387</v>
+      </c>
+      <c r="E31" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="22">
         <v>11726</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="22">
         <v>11726</v>
       </c>
     </row>
@@ -6203,22 +6311,22 @@
       <c r="B32" s="7">
         <v>30</v>
       </c>
-      <c r="C32" s="16">
-        <f t="shared" si="8"/>
-        <v>3.501835168501835</v>
-      </c>
-      <c r="D32" s="16">
+      <c r="C32" s="20">
         <f t="shared" si="9"/>
         <v>3.501835168501835</v>
       </c>
-      <c r="E32" s="16">
-        <f>ABS(C32-D32)</f>
+      <c r="D32" s="20">
+        <f t="shared" si="10"/>
+        <v>3.501835168501835</v>
+      </c>
+      <c r="E32" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="22">
         <v>11988</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="22">
         <v>11988</v>
       </c>
     </row>
@@ -6226,46 +6334,46 @@
       <c r="B33" s="7">
         <v>31</v>
       </c>
-      <c r="C33" s="16">
-        <f t="shared" si="8"/>
+      <c r="C33" s="20">
+        <f t="shared" si="9"/>
         <v>3.5960253554908341</v>
       </c>
-      <c r="D33" s="16">
-        <f t="shared" si="9"/>
+      <c r="D33" s="20">
+        <f t="shared" si="10"/>
         <v>3.5978745286253</v>
       </c>
-      <c r="E33" s="16">
-        <f>ABS(C33-D33)</f>
+      <c r="E33" s="20">
+        <f t="shared" si="11"/>
         <v>0.0018491731344658646</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="22">
         <v>11674</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="22">
         <v>11668</v>
       </c>
-      <c r="L33" s="15"/>
+      <c r="L33" s="23"/>
     </row>
     <row r="34">
       <c r="B34" s="7">
         <v>32</v>
       </c>
-      <c r="C34" s="16">
-        <f t="shared" si="8"/>
+      <c r="C34" s="20">
+        <f t="shared" si="9"/>
         <v>3.5221075593590068</v>
       </c>
-      <c r="D34" s="16">
-        <f t="shared" si="9"/>
+      <c r="D34" s="20">
+        <f t="shared" si="10"/>
         <v>3.5218120805369129</v>
       </c>
-      <c r="E34" s="16">
-        <f>ABS(C34-D34)</f>
+      <c r="E34" s="20">
+        <f t="shared" si="11"/>
         <v>0.00029547882209390863</v>
       </c>
-      <c r="F34" s="14">
+      <c r="F34" s="22">
         <v>11919</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="22">
         <v>11920</v>
       </c>
     </row>
@@ -6273,22 +6381,22 @@
       <c r="B35" s="7">
         <v>33</v>
       </c>
-      <c r="C35" s="16">
-        <f t="shared" si="8"/>
-        <v>3.6174062903920725</v>
-      </c>
-      <c r="D35" s="16">
+      <c r="C35" s="20">
         <f t="shared" si="9"/>
         <v>3.6174062903920725</v>
       </c>
-      <c r="E35" s="16">
-        <f>ABS(C35-D35)</f>
+      <c r="D35" s="20">
+        <f t="shared" si="10"/>
+        <v>3.6174062903920725</v>
+      </c>
+      <c r="E35" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F35" s="21">
         <v>11605</v>
       </c>
-      <c r="G35" s="11">
+      <c r="G35" s="21">
         <v>11605</v>
       </c>
     </row>
@@ -6296,22 +6404,22 @@
       <c r="B36" s="7">
         <v>34</v>
       </c>
-      <c r="C36" s="16">
-        <f t="shared" si="8"/>
+      <c r="C36" s="20">
+        <f t="shared" si="9"/>
         <v>3.5423171040418531</v>
       </c>
-      <c r="D36" s="16">
-        <f t="shared" si="9"/>
+      <c r="D36" s="20">
+        <f t="shared" si="10"/>
         <v>3.5396290050590218</v>
       </c>
-      <c r="E36" s="16">
-        <f>ABS(C36-D36)</f>
+      <c r="E36" s="20">
+        <f t="shared" si="11"/>
         <v>0.0026880989828312885</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="21">
         <v>11851</v>
       </c>
-      <c r="G36" s="11">
+      <c r="G36" s="21">
         <v>11860</v>
       </c>
     </row>
@@ -6319,22 +6427,22 @@
       <c r="B37" s="7">
         <v>35</v>
       </c>
-      <c r="C37" s="16">
-        <f t="shared" si="8"/>
+      <c r="C37" s="20">
+        <f t="shared" si="9"/>
         <v>3.6227131515360718</v>
       </c>
-      <c r="D37" s="16">
-        <f t="shared" si="9"/>
+      <c r="D37" s="20">
+        <f t="shared" si="10"/>
         <v>3.6233385119972379</v>
       </c>
-      <c r="E37" s="16">
-        <f>ABS(C37-D37)</f>
+      <c r="E37" s="20">
+        <f t="shared" si="11"/>
         <v>0.00062536046116612454</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F37" s="21">
         <v>11588</v>
       </c>
-      <c r="G37" s="11">
+      <c r="G37" s="21">
         <v>11586</v>
       </c>
     </row>
@@ -6342,22 +6450,22 @@
       <c r="B38" s="7">
         <v>36</v>
       </c>
-      <c r="C38" s="16">
-        <f t="shared" si="8"/>
+      <c r="C38" s="20">
+        <f t="shared" si="9"/>
         <v>3.5558190750465863</v>
       </c>
-      <c r="D38" s="16">
-        <f t="shared" si="9"/>
+      <c r="D38" s="20">
+        <f t="shared" si="10"/>
         <v>3.557627118644068</v>
       </c>
-      <c r="E38" s="16">
-        <f>ABS(C38-D38)</f>
+      <c r="E38" s="20">
+        <f t="shared" si="11"/>
         <v>0.0018080435974816567</v>
       </c>
-      <c r="F38" s="11">
+      <c r="F38" s="21">
         <v>11806</v>
       </c>
-      <c r="G38" s="11">
+      <c r="G38" s="21">
         <v>11800</v>
       </c>
     </row>
@@ -6365,22 +6473,22 @@
       <c r="B39" s="7">
         <v>37</v>
       </c>
-      <c r="C39" s="16">
-        <f t="shared" si="8"/>
+      <c r="C39" s="20">
+        <f t="shared" si="9"/>
         <v>3.6380968888118557</v>
       </c>
-      <c r="D39" s="16">
-        <f t="shared" si="9"/>
+      <c r="D39" s="20">
+        <f t="shared" si="10"/>
         <v>3.6384122031547927</v>
       </c>
-      <c r="E39" s="16">
-        <f>ABS(C39-D39)</f>
+      <c r="E39" s="20">
+        <f t="shared" si="11"/>
         <v>0.00031531434293707861</v>
       </c>
-      <c r="F39" s="11">
+      <c r="F39" s="21">
         <v>11539</v>
       </c>
-      <c r="G39" s="11">
+      <c r="G39" s="21">
         <v>11538</v>
       </c>
     </row>
@@ -6388,22 +6496,22 @@
       <c r="B40" s="7">
         <v>38</v>
       </c>
-      <c r="C40" s="16">
-        <f t="shared" si="8"/>
+      <c r="C40" s="20">
+        <f t="shared" si="9"/>
         <v>3.5724619181346267</v>
       </c>
-      <c r="D40" s="16">
-        <f t="shared" si="9"/>
+      <c r="D40" s="20">
+        <f t="shared" si="10"/>
         <v>3.5730700485147673</v>
       </c>
-      <c r="E40" s="16">
-        <f>ABS(C40-D40)</f>
+      <c r="E40" s="20">
+        <f t="shared" si="11"/>
         <v>0.0006081303801406257</v>
       </c>
-      <c r="F40" s="11">
+      <c r="F40" s="21">
         <v>11751</v>
       </c>
-      <c r="G40" s="11">
+      <c r="G40" s="21">
         <v>11749</v>
       </c>
     </row>
@@ -6411,22 +6519,22 @@
       <c r="B41" s="7">
         <v>39</v>
       </c>
-      <c r="C41" s="16">
-        <f t="shared" si="8"/>
+      <c r="C41" s="20">
+        <f t="shared" si="9"/>
         <v>3.6501173810972958</v>
       </c>
-      <c r="D41" s="16">
-        <f t="shared" si="9"/>
+      <c r="D41" s="20">
+        <f t="shared" si="10"/>
         <v>3.6447299878451118</v>
       </c>
-      <c r="E41" s="16">
-        <f>ABS(C41-D41)</f>
+      <c r="E41" s="20">
+        <f t="shared" si="11"/>
         <v>0.0053873932521839585</v>
       </c>
-      <c r="F41" s="11">
+      <c r="F41" s="21">
         <v>11501</v>
       </c>
-      <c r="G41" s="11">
+      <c r="G41" s="21">
         <v>11518</v>
       </c>
     </row>
@@ -6434,22 +6542,22 @@
       <c r="B42" s="7">
         <v>40</v>
       </c>
-      <c r="C42" s="16">
-        <f t="shared" si="8"/>
+      <c r="C42" s="20">
+        <f t="shared" si="9"/>
         <v>3.5809946259489891</v>
       </c>
-      <c r="D42" s="16">
-        <f t="shared" si="9"/>
+      <c r="D42" s="20">
+        <f t="shared" si="10"/>
         <v>3.5828283690364429</v>
       </c>
-      <c r="E42" s="16">
-        <f>ABS(C42-D42)</f>
+      <c r="E42" s="20">
+        <f t="shared" si="11"/>
         <v>0.0018337430874537652</v>
       </c>
-      <c r="F42" s="11">
+      <c r="F42" s="21">
         <v>11723</v>
       </c>
-      <c r="G42" s="11">
+      <c r="G42" s="21">
         <v>11717</v>
       </c>
     </row>
@@ -6457,22 +6565,22 @@
       <c r="B43" s="7">
         <v>41</v>
       </c>
-      <c r="C43" s="16">
-        <f t="shared" si="8"/>
+      <c r="C43" s="20">
+        <f t="shared" si="9"/>
         <v>3.6571129889363183</v>
       </c>
-      <c r="D43" s="16">
-        <f t="shared" si="9"/>
+      <c r="D43" s="20">
+        <f t="shared" si="10"/>
         <v>3.6567944250871078</v>
       </c>
-      <c r="E43" s="16">
-        <f>ABS(C43-D43)</f>
+      <c r="E43" s="20">
+        <f t="shared" si="11"/>
         <v>0.00031856384921047365</v>
       </c>
-      <c r="F43" s="11">
+      <c r="F43" s="21">
         <v>11479</v>
       </c>
-      <c r="G43" s="11">
+      <c r="G43" s="21">
         <v>11480</v>
       </c>
     </row>
@@ -6480,22 +6588,22 @@
       <c r="B44" s="7">
         <v>42</v>
       </c>
-      <c r="C44" s="16">
-        <f t="shared" si="8"/>
-        <v>3.5923327058018142</v>
-      </c>
-      <c r="D44" s="16">
+      <c r="C44" s="20">
         <f t="shared" si="9"/>
         <v>3.5923327058018142</v>
       </c>
-      <c r="E44" s="16">
-        <f>ABS(C44-D44)</f>
+      <c r="D44" s="20">
+        <f t="shared" si="10"/>
+        <v>3.5923327058018142</v>
+      </c>
+      <c r="E44" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F44" s="11">
+      <c r="F44" s="21">
         <v>11686</v>
       </c>
-      <c r="G44" s="11">
+      <c r="G44" s="21">
         <v>11686</v>
       </c>
     </row>
@@ -6503,22 +6611,22 @@
       <c r="B45" s="7">
         <v>43</v>
       </c>
-      <c r="C45" s="16">
-        <f t="shared" si="8"/>
-        <v>3.6634959420542805</v>
-      </c>
-      <c r="D45" s="16">
+      <c r="C45" s="20">
         <f t="shared" si="9"/>
         <v>3.6634959420542805</v>
       </c>
-      <c r="E45" s="16">
-        <f>ABS(C45-D45)</f>
+      <c r="D45" s="20">
+        <f t="shared" si="10"/>
+        <v>3.6634959420542805</v>
+      </c>
+      <c r="E45" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F45" s="11">
+      <c r="F45" s="21">
         <v>11459</v>
       </c>
-      <c r="G45" s="11">
+      <c r="G45" s="21">
         <v>11459</v>
       </c>
     </row>
@@ -6526,22 +6634,22 @@
       <c r="B46" s="7">
         <v>44</v>
       </c>
-      <c r="C46" s="16">
-        <f t="shared" si="8"/>
-        <v>3.6043616381900918</v>
-      </c>
-      <c r="D46" s="16">
+      <c r="C46" s="20">
         <f t="shared" si="9"/>
         <v>3.6043616381900918</v>
       </c>
-      <c r="E46" s="16">
-        <f>ABS(C46-D46)</f>
+      <c r="D46" s="20">
+        <f t="shared" si="10"/>
+        <v>3.6043616381900918</v>
+      </c>
+      <c r="E46" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F46" s="11">
+      <c r="F46" s="21">
         <v>11647</v>
       </c>
-      <c r="G46" s="11">
+      <c r="G46" s="21">
         <v>11647</v>
       </c>
     </row>
@@ -6549,22 +6657,22 @@
       <c r="B47" s="7">
         <v>45</v>
       </c>
-      <c r="C47" s="16">
-        <f t="shared" si="8"/>
+      <c r="C47" s="20">
+        <f t="shared" si="9"/>
         <v>3.6708639384400139</v>
       </c>
-      <c r="D47" s="16">
-        <f t="shared" si="9"/>
+      <c r="D47" s="20">
+        <f t="shared" si="10"/>
         <v>3.6692596800978934</v>
       </c>
-      <c r="E47" s="16">
-        <f>ABS(C47-D47)</f>
+      <c r="E47" s="20">
+        <f t="shared" si="11"/>
         <v>0.0016042583421205237</v>
       </c>
-      <c r="F47" s="11">
+      <c r="F47" s="21">
         <v>11436</v>
       </c>
-      <c r="G47" s="11">
+      <c r="G47" s="21">
         <v>11441</v>
       </c>
     </row>
@@ -6572,22 +6680,22 @@
       <c r="B48" s="7">
         <v>46</v>
       </c>
-      <c r="C48" s="16">
-        <f t="shared" si="8"/>
+      <c r="C48" s="20">
+        <f t="shared" si="9"/>
         <v>3.6164713990351482</v>
       </c>
-      <c r="D48" s="16">
-        <f t="shared" si="9"/>
+      <c r="D48" s="20">
+        <f t="shared" si="10"/>
         <v>3.6155369907846007</v>
       </c>
-      <c r="E48" s="16">
-        <f>ABS(C48-D48)</f>
+      <c r="E48" s="20">
+        <f t="shared" si="11"/>
         <v>0.00093440825054758037</v>
       </c>
-      <c r="F48" s="11">
+      <c r="F48" s="21">
         <v>11608</v>
       </c>
-      <c r="G48" s="11">
+      <c r="G48" s="21">
         <v>11611</v>
       </c>
     </row>
@@ -6595,22 +6703,22 @@
       <c r="B49" s="7">
         <v>47</v>
       </c>
-      <c r="C49" s="16">
-        <f t="shared" si="8"/>
+      <c r="C49" s="20">
+        <f t="shared" si="9"/>
         <v>3.676650902084428</v>
       </c>
-      <c r="D49" s="16">
-        <f t="shared" si="9"/>
+      <c r="D49" s="20">
+        <f t="shared" si="10"/>
         <v>3.6702220667948944</v>
       </c>
-      <c r="E49" s="16">
-        <f>ABS(C49-D49)</f>
+      <c r="E49" s="20">
+        <f t="shared" si="11"/>
         <v>0.0064288352895336409</v>
       </c>
-      <c r="F49" s="11">
+      <c r="F49" s="21">
         <v>11418</v>
       </c>
-      <c r="G49" s="11">
+      <c r="G49" s="21">
         <v>11438</v>
       </c>
     </row>
@@ -6618,22 +6726,22 @@
       <c r="B50" s="7">
         <v>48</v>
       </c>
-      <c r="C50" s="16">
-        <f t="shared" si="8"/>
-        <v>3.6220880069025023</v>
-      </c>
-      <c r="D50" s="16">
+      <c r="C50" s="20">
         <f t="shared" si="9"/>
         <v>3.6220880069025023</v>
       </c>
-      <c r="E50" s="16">
-        <f>ABS(C50-D50)</f>
+      <c r="D50" s="20">
+        <f t="shared" si="10"/>
+        <v>3.6220880069025023</v>
+      </c>
+      <c r="E50" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F50" s="11">
+      <c r="F50" s="21">
         <v>11590</v>
       </c>
-      <c r="G50" s="11">
+      <c r="G50" s="21">
         <v>11590</v>
       </c>
     </row>
@@ -6641,22 +6749,22 @@
       <c r="B51" s="7">
         <v>49</v>
       </c>
-      <c r="C51" s="16">
-        <f t="shared" si="8"/>
+      <c r="C51" s="20">
+        <f t="shared" si="9"/>
         <v>3.6792287467134095</v>
       </c>
-      <c r="D51" s="16">
-        <f t="shared" si="9"/>
+      <c r="D51" s="20">
+        <f t="shared" si="10"/>
         <v>3.6795512314839161</v>
       </c>
-      <c r="E51" s="16">
-        <f>ABS(C51-D51)</f>
+      <c r="E51" s="20">
+        <f t="shared" si="11"/>
         <v>0.00032248477050655922</v>
       </c>
-      <c r="F51" s="11">
+      <c r="F51" s="21">
         <v>11410</v>
       </c>
-      <c r="G51" s="11">
+      <c r="G51" s="21">
         <v>11409</v>
       </c>
     </row>
@@ -6664,22 +6772,22 @@
       <c r="B52" s="7">
         <v>50</v>
       </c>
-      <c r="C52" s="16">
-        <f t="shared" si="8"/>
+      <c r="C52" s="20">
+        <f t="shared" si="9"/>
         <v>3.6242769576102911</v>
       </c>
-      <c r="D52" s="16">
-        <f t="shared" si="9"/>
+      <c r="D52" s="20">
+        <f t="shared" si="10"/>
         <v>3.625842114354811</v>
       </c>
-      <c r="E52" s="16">
-        <f>ABS(C52-D52)</f>
+      <c r="E52" s="20">
+        <f t="shared" si="11"/>
         <v>0.0015651567445198467</v>
       </c>
-      <c r="F52" s="11">
+      <c r="F52" s="21">
         <v>11583</v>
       </c>
-      <c r="G52" s="11">
+      <c r="G52" s="21">
         <v>11578</v>
       </c>
     </row>
@@ -6687,22 +6795,22 @@
       <c r="B53" s="7">
         <v>51</v>
       </c>
-      <c r="C53" s="16">
-        <f t="shared" si="8"/>
+      <c r="C53" s="20">
+        <f t="shared" si="9"/>
         <v>3.6843952957697033</v>
       </c>
-      <c r="D53" s="16">
-        <f t="shared" si="9"/>
+      <c r="D53" s="20">
+        <f t="shared" si="10"/>
         <v>3.6840719613865729</v>
       </c>
-      <c r="E53" s="16">
-        <f>ABS(C53-D53)</f>
+      <c r="E53" s="20">
+        <f t="shared" si="11"/>
         <v>0.00032333438313036922</v>
       </c>
-      <c r="F53" s="11">
+      <c r="F53" s="21">
         <v>11394</v>
       </c>
-      <c r="G53" s="11">
+      <c r="G53" s="21">
         <v>11395</v>
       </c>
     </row>
@@ -6710,22 +6818,22 @@
       <c r="B54" s="7">
         <v>52</v>
       </c>
-      <c r="C54" s="16">
-        <f t="shared" si="8"/>
+      <c r="C54" s="20">
+        <f t="shared" si="9"/>
         <v>3.6327448944271374</v>
       </c>
-      <c r="D54" s="16">
-        <f t="shared" si="9"/>
+      <c r="D54" s="20">
+        <f t="shared" si="10"/>
         <v>3.6324305615644197</v>
       </c>
-      <c r="E54" s="16">
-        <f>ABS(C54-D54)</f>
+      <c r="E54" s="20">
+        <f t="shared" si="11"/>
         <v>0.00031433286271775884</v>
       </c>
-      <c r="F54" s="11">
+      <c r="F54" s="21">
         <v>11556</v>
       </c>
-      <c r="G54" s="11">
+      <c r="G54" s="21">
         <v>11557</v>
       </c>
     </row>
@@ -6733,22 +6841,22 @@
       <c r="B55" s="7">
         <v>53</v>
       </c>
-      <c r="C55" s="16">
-        <f t="shared" si="8"/>
+      <c r="C55" s="20">
+        <f t="shared" si="9"/>
         <v>3.6899006768040783</v>
       </c>
-      <c r="D55" s="16">
-        <f t="shared" si="9"/>
+      <c r="D55" s="20">
+        <f t="shared" si="10"/>
         <v>3.6905494505494505</v>
       </c>
-      <c r="E55" s="16">
-        <f>ABS(C55-D55)</f>
+      <c r="E55" s="20">
+        <f t="shared" si="11"/>
         <v>0.00064877374537219978</v>
       </c>
-      <c r="F55" s="11">
+      <c r="F55" s="21">
         <v>11377</v>
       </c>
-      <c r="G55" s="11">
+      <c r="G55" s="21">
         <v>11375</v>
       </c>
     </row>
@@ -6756,22 +6864,22 @@
       <c r="B56" s="7">
         <v>54</v>
       </c>
-      <c r="C56" s="16">
-        <f t="shared" si="8"/>
-        <v>3.6393584742089296</v>
-      </c>
-      <c r="D56" s="16">
+      <c r="C56" s="20">
         <f t="shared" si="9"/>
         <v>3.6393584742089296</v>
       </c>
-      <c r="E56" s="16">
-        <f>ABS(C56-D56)</f>
+      <c r="D56" s="20">
+        <f t="shared" si="10"/>
+        <v>3.6393584742089296</v>
+      </c>
+      <c r="E56" s="20">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="F56" s="11">
+      <c r="F56" s="21">
         <v>11535</v>
       </c>
-      <c r="G56" s="11">
+      <c r="G56" s="21">
         <v>11535</v>
       </c>
     </row>
@@ -6779,22 +6887,22 @@
       <c r="B57" s="7">
         <v>55</v>
       </c>
-      <c r="C57" s="17">
-        <f t="shared" si="8"/>
+      <c r="C57" s="24">
+        <f t="shared" si="9"/>
         <v>3.6947720471747934</v>
       </c>
-      <c r="D57" s="16">
-        <f t="shared" si="9"/>
+      <c r="D57" s="20">
+        <f t="shared" si="10"/>
         <v>3.6954225352112675</v>
       </c>
-      <c r="E57" s="16">
-        <f>ABS(C57-D57)</f>
+      <c r="E57" s="20">
+        <f t="shared" si="11"/>
         <v>0.00065048803647416165</v>
       </c>
-      <c r="F57" s="14">
+      <c r="F57" s="22">
         <v>11362</v>
       </c>
-      <c r="G57" s="11">
+      <c r="G57" s="21">
         <v>11360</v>
       </c>
     </row>
@@ -6802,22 +6910,22 @@
       <c r="B58" s="7">
         <v>56</v>
       </c>
-      <c r="C58" s="17">
-        <f t="shared" si="8"/>
+      <c r="C58" s="24">
+        <f t="shared" si="9"/>
         <v>3.6459961785652251</v>
       </c>
-      <c r="D58" s="16">
-        <f t="shared" si="9"/>
+      <c r="D58" s="20">
+        <f t="shared" si="10"/>
         <v>3.6472632493483927</v>
       </c>
-      <c r="E58" s="16">
-        <f>ABS(C58-D58)</f>
+      <c r="E58" s="20">
+        <f t="shared" si="11"/>
         <v>0.0012670707831676786</v>
       </c>
-      <c r="F58" s="14">
+      <c r="F58" s="22">
         <v>11514</v>
       </c>
-      <c r="G58" s="11">
+      <c r="G58" s="21">
         <v>11510</v>
       </c>
     </row>
@@ -6825,22 +6933,22 @@
       <c r="B59" s="7">
         <v>57</v>
       </c>
-      <c r="C59" s="17">
-        <f t="shared" si="8"/>
+      <c r="C59" s="24">
+        <f t="shared" si="9"/>
         <v>3.6977010481810977</v>
       </c>
-      <c r="D59" s="16">
-        <f t="shared" si="9"/>
+      <c r="D59" s="20">
+        <f t="shared" si="10"/>
         <v>3.6963986968389539</v>
       </c>
-      <c r="E59" s="16">
-        <f>ABS(C59-D59)</f>
+      <c r="E59" s="20">
+        <f t="shared" si="11"/>
         <v>0.0013023513421437372</v>
       </c>
-      <c r="F59" s="14">
+      <c r="F59" s="22">
         <v>11353</v>
       </c>
-      <c r="G59" s="11">
+      <c r="G59" s="21">
         <v>11357</v>
       </c>
     </row>
@@ -6848,22 +6956,22 @@
       <c r="B60" s="7">
         <v>58</v>
       </c>
-      <c r="C60" s="17">
-        <f t="shared" si="8"/>
+      <c r="C60" s="24">
+        <f t="shared" si="9"/>
         <v>3.6501173810972958</v>
       </c>
-      <c r="D60" s="16">
-        <f t="shared" si="9"/>
+      <c r="D60" s="20">
+        <f t="shared" si="10"/>
         <v>3.6485312011124629</v>
       </c>
-      <c r="E60" s="16">
-        <f>ABS(C60-D60)</f>
+      <c r="E60" s="20">
+        <f t="shared" si="11"/>
         <v>0.0015861799848329028</v>
       </c>
-      <c r="F60" s="14">
+      <c r="F60" s="22">
         <v>11501</v>
       </c>
-      <c r="G60" s="14">
+      <c r="G60" s="22">
         <v>11506</v>
       </c>
     </row>
@@ -6871,22 +6979,22 @@
       <c r="B61" s="7">
         <v>59</v>
       </c>
-      <c r="C61" s="17">
-        <f t="shared" si="8"/>
+      <c r="C61" s="24">
+        <f t="shared" si="9"/>
         <v>3.6986784140969164</v>
       </c>
-      <c r="D61" s="16">
-        <f t="shared" si="9"/>
+      <c r="D61" s="20">
+        <f t="shared" si="10"/>
         <v>3.6983525680556779</v>
       </c>
-      <c r="E61" s="16">
-        <f>ABS(C61-D61)</f>
+      <c r="E61" s="20">
+        <f t="shared" si="11"/>
         <v>0.00032584604123853111</v>
       </c>
-      <c r="F61" s="14">
+      <c r="F61" s="22">
         <v>11350</v>
       </c>
-      <c r="G61" s="14">
+      <c r="G61" s="22">
         <v>11351</v>
       </c>
     </row>
@@ -6894,22 +7002,22 @@
       <c r="B62" s="7">
         <v>60</v>
       </c>
-      <c r="C62" s="17">
-        <f t="shared" si="8"/>
+      <c r="C62" s="24">
+        <f t="shared" si="9"/>
         <v>3.6529759832927255</v>
       </c>
-      <c r="D62" s="16">
-        <f t="shared" si="9"/>
+      <c r="D62" s="20">
+        <f t="shared" si="10"/>
         <v>3.6520226185297955</v>
       </c>
-      <c r="E62" s="16">
-        <f>ABS(C62-D62)</f>
+      <c r="E62" s="20">
+        <f t="shared" si="11"/>
         <v>0.00095336476293006456</v>
       </c>
-      <c r="F62" s="14">
+      <c r="F62" s="22">
         <v>11492</v>
       </c>
-      <c r="G62" s="14">
+      <c r="G62" s="22">
         <v>11495</v>
       </c>
     </row>
@@ -6917,22 +7025,22 @@
       <c r="B63" s="7">
         <v>61</v>
       </c>
-      <c r="C63" s="17">
-        <f t="shared" si="8"/>
+      <c r="C63" s="24">
+        <f t="shared" si="9"/>
         <v>3.6980267794221282</v>
       </c>
-      <c r="D63" s="16">
-        <f t="shared" si="9"/>
+      <c r="D63" s="20">
+        <f t="shared" si="10"/>
         <v>3.7009609450762584</v>
       </c>
-      <c r="E63" s="16">
-        <f>ABS(C63-D63)</f>
+      <c r="E63" s="20">
+        <f t="shared" si="11"/>
         <v>0.002934165654130183</v>
       </c>
-      <c r="F63" s="14">
+      <c r="F63" s="22">
         <v>11352</v>
       </c>
-      <c r="G63" s="14">
+      <c r="G63" s="22">
         <v>11343</v>
       </c>
     </row>
@@ -6940,22 +7048,22 @@
       <c r="B64" s="7">
         <v>62</v>
       </c>
-      <c r="C64" s="17">
-        <f t="shared" si="8"/>
+      <c r="C64" s="24">
+        <f t="shared" si="9"/>
         <v>3.6571129889363183</v>
       </c>
-      <c r="D64" s="16">
-        <f t="shared" si="9"/>
+      <c r="D64" s="20">
+        <f t="shared" si="10"/>
         <v>3.6548842068605261</v>
       </c>
-      <c r="E64" s="16">
-        <f>ABS(C64-D64)</f>
+      <c r="E64" s="20">
+        <f t="shared" si="11"/>
         <v>0.0022287820757922461</v>
       </c>
-      <c r="F64" s="14">
+      <c r="F64" s="22">
         <v>11479</v>
       </c>
-      <c r="G64" s="14">
+      <c r="G64" s="22">
         <v>11486</v>
       </c>
     </row>
@@ -6963,22 +7071,22 @@
       <c r="B65" s="7">
         <v>63</v>
       </c>
-      <c r="C65" s="17">
-        <f t="shared" si="8"/>
+      <c r="C65" s="24">
+        <f t="shared" si="9"/>
         <v>3.7003085059497578</v>
       </c>
-      <c r="D65" s="16">
-        <f t="shared" si="9"/>
+      <c r="D65" s="20">
+        <f t="shared" si="10"/>
         <v>3.6999823726423409</v>
       </c>
-      <c r="E65" s="16">
-        <f>ABS(C65-D65)</f>
+      <c r="E65" s="20">
+        <f t="shared" si="11"/>
         <v>0.00032613330741693147</v>
       </c>
-      <c r="F65" s="14">
+      <c r="F65" s="22">
         <v>11345</v>
       </c>
-      <c r="G65" s="14">
+      <c r="G65" s="22">
         <v>11346</v>
       </c>
     </row>
@@ -6986,22 +7094,22 @@
       <c r="B66" s="7">
         <v>64</v>
       </c>
-      <c r="C66" s="17">
-        <f t="shared" si="8"/>
+      <c r="C66" s="24">
+        <f t="shared" si="9"/>
         <v>3.6599825632083696</v>
       </c>
-      <c r="D66" s="16">
-        <f t="shared" si="9"/>
+      <c r="D66" s="20">
+        <f t="shared" si="10"/>
         <v>3.6590255382201691</v>
       </c>
-      <c r="E66" s="16">
-        <f>ABS(C66-D66)</f>
+      <c r="E66" s="20">
+        <f t="shared" si="11"/>
         <v>0.00095702498820049442</v>
       </c>
-      <c r="F66" s="14">
+      <c r="F66" s="22">
         <v>11470</v>
       </c>
-      <c r="G66" s="14">
+      <c r="G66" s="22">
         <v>11473</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated evaluation, fixed core assign
</commit_message>
<xml_diff>
--- a/documentation/evaluation-2019-11-18.xlsx
+++ b/documentation/evaluation-2019-11-18.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="8 threads" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">number of threads</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">execution time (ms) [2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total speedup [3]</t>
   </si>
   <si>
     <r>
@@ -87,6 +90,9 @@
       </rPr>
       <t>|</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">execution time (ms) [3]</t>
   </si>
 </sst>
 </file>
@@ -2722,22 +2728,237 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLeaderLines val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f xml:space="preserve">'64 threads'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v xml:space="preserve">total speedup [3]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f xml:space="preserve">'64 threads'!$E$3:$E$66</c:f>
+              <c:numCache>
+                <c:ptCount val="64"/>
+                <c:pt idx="0" formatCode="0.000">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="0.000">
+                  <c:v>2.0002378573807147</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000">
+                  <c:v>2.0002378573807147</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.000">
+                  <c:v>2.666603247082699</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.000">
+                  <c:v>2.5004162702188393</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.000">
+                  <c:v>3.000570898451438</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.000">
+                  <c:v>2.800519515119222</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.000">
+                  <c:v>3.199193487027315</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.000">
+                  <c:v>2.9986449864498645</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.000">
+                  <c:v>3.329927932208759</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.000">
+                  <c:v>3.1399447390038087</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.000">
+                  <c:v>3.422072108732807</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.000">
+                  <c:v>3.244617640250019</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.000">
+                  <c:v>3.489667192298116</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.000">
+                  <c:v>3.3241362953593168</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.000">
+                  <c:v>3.54169474393531</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.000">
+                  <c:v>3.386244664572763</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.000">
+                  <c:v>3.581516183986371</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="0.000">
+                  <c:v>3.4374591236102026</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0.000">
+                  <c:v>3.6132164647245855</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="0.000">
+                  <c:v>3.4810000827883103</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0.000">
+                  <c:v>3.6394875789838137</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0.000">
+                  <c:v>3.5147538242915655</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="0.000">
+                  <c:v>3.661036134087941</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="0.000">
+                  <c:v>3.5425899401803016</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="0.000">
+                  <c:v>3.678652668416448</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="0.000">
+                  <c:v>3.5708704883227176</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="0.000">
+                  <c:v>3.6902755836405126</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="0.000">
+                  <c:v>3.589772048151626</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="0.000">
+                  <c:v>3.7039288231148695</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="0.000">
+                  <c:v>3.6088747746974508</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="0.000">
+                  <c:v>3.7166976045257667</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="0.000">
+                  <c:v>3.623804188571921</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="0.000">
+                  <c:v>3.7305474225889452</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0.000">
+                  <c:v>3.638227913818465</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0.000">
+                  <c:v>3.733197194353192</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0.000">
+                  <c:v>3.6502300546922477</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0.000">
+                  <c:v>3.738840476613907</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="0.000">
+                  <c:v>3.6578512396694216</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="0.000">
+                  <c:v>3.744500846023689</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="0.000">
+                  <c:v>3.668702556495943</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="0.000">
+                  <c:v>3.749175211769951</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="0.000">
+                  <c:v>3.6764011541488153</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="0.000">
+                  <c:v>3.7562086832231554</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="0.000">
+                  <c:v>3.678652668416448</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="0.000">
+                  <c:v>3.752186328752454</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="0.000">
+                  <c:v>3.6851007887817704</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="0.000">
+                  <c:v>3.7582230961744725</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="0.000">
+                  <c:v>3.6909234550561796</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="0.000">
+                  <c:v>3.762258410880458</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="0.000">
+                  <c:v>3.697089598171107</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="0.000">
+                  <c:v>3.7585590417448826</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="0.000">
+                  <c:v>3.706214191273689</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="0.000">
+                  <c:v>3.7548669405250936</c:v>
+                </c:pt>
+                <c:pt idx="54" formatCode="0.000">
+                  <c:v>3.704581497797357</c:v>
+                </c:pt>
+                <c:pt idx="55" formatCode="0.000">
+                  <c:v>3.759231113097899</c:v>
+                </c:pt>
+                <c:pt idx="56" formatCode="0.000">
+                  <c:v>3.707848324514991</c:v>
+                </c:pt>
+                <c:pt idx="57" formatCode="0.000">
+                  <c:v>3.7673147567422274</c:v>
+                </c:pt>
+                <c:pt idx="58" formatCode="0.000">
+                  <c:v>3.7137431549196256</c:v>
+                </c:pt>
+                <c:pt idx="59" formatCode="0.000">
+                  <c:v>3.7666397921705634</c:v>
+                </c:pt>
+                <c:pt idx="60" formatCode="0.000">
+                  <c:v>3.714727449421327</c:v>
+                </c:pt>
+                <c:pt idx="61" formatCode="0.000">
+                  <c:v>3.762258410880458</c:v>
+                </c:pt>
+                <c:pt idx="62" formatCode="0.000">
+                  <c:v>3.7180122026704394</c:v>
+                </c:pt>
+                <c:pt idx="63" formatCode="0.000">
+                  <c:v>3.767652329749104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1035"/>
-        <c:axId val="1036"/>
+        <c:axId val="1007"/>
+        <c:axId val="1008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1035"/>
+        <c:axId val="1007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2805,8 +3026,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1036"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="1008"/>
         <c:crossesAt val="0.5"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2815,10 +3035,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1036"/>
+        <c:axId val="1008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2907,7 +3127,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1035"/>
+        <c:crossAx val="1007"/>
         <c:crosses val="min"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2932,7 +3152,7 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm>
-      <a:off x="10067924" y="182540"/>
+      <a:off x="14192248" y="182539"/>
       <a:ext cx="7858123" cy="5294333"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
@@ -3060,11 +3280,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f xml:space="preserve">'64 threads'!$E$2</c:f>
+              <c:f xml:space="preserve">'64 threads'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v xml:space="preserve">| ttotal speedup [1] - ttotal speedup [2] |</c:v>
+                  <c:v xml:space="preserve">| tS[1] - tS[2] |</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3079,7 +3299,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f xml:space="preserve">'64 threads'!$E$3:$E$66</c:f>
+              <c:f xml:space="preserve">'64 threads'!$F$3:$F$66</c:f>
               <c:numCache>
                 <c:ptCount val="64"/>
                 <c:pt idx="0" formatCode="0.000">
@@ -3279,21 +3499,13 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
-        </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1025"/>
-        <c:axId val="1026"/>
+        <c:axId val="1005"/>
+        <c:axId val="1006"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1025"/>
+        <c:axId val="1005"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3361,8 +3573,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1026"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="1006"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3371,7 +3582,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1026"/>
+        <c:axId val="1006"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.01"/>
@@ -3405,13 +3616,13 @@
                     <a:spcPts val="0"/>
                   </a:spcBef>
                   <a:spcAft>
-                    <a:spcPts val="539"/>
+                    <a:spcPts val="538"/>
                   </a:spcAft>
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
                   <a:rPr/>
-                  <a:t>Δt  in  ms</a:t>
+                  <a:t>ΔSpeedup</a:t>
                 </a:r>
                 <a:endParaRPr/>
               </a:p>
@@ -3458,7 +3669,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1025"/>
+        <c:crossAx val="1005"/>
         <c:crosses val="min"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3483,7 +3694,7 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm>
-      <a:off x="10058399" y="5943599"/>
+      <a:off x="14182723" y="5943598"/>
       <a:ext cx="7858122" cy="5294332"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
@@ -3637,7 +3848,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>600073</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1564</xdr:rowOff>
+      <xdr:rowOff>1563</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
@@ -3671,16 +3882,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9523</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1565</xdr:rowOff>
+      <xdr:rowOff>1564</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>552448</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>552446</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:rowOff>19047</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3690,7 +3901,7 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10067924" y="182540"/>
+        <a:off x="14192248" y="182539"/>
         <a:ext cx="7858123" cy="5294333"/>
       </xdr:xfrm>
       <a:graphic>
@@ -3703,16 +3914,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>609598</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:rowOff>123823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>542922</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>542920</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>169882</xdr:rowOff>
+      <xdr:rowOff>169880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3722,7 +3933,7 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10058399" y="5943599"/>
+        <a:off x="14182723" y="5943598"/>
         <a:ext cx="7858122" cy="5294332"/>
       </xdr:xfrm>
       <a:graphic>
@@ -5617,11 +5828,15 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="3.421875"/>
     <col customWidth="1" min="2" max="2" width="22.7109375"/>
-    <col customWidth="1" min="3" max="4" width="18.421875"/>
-    <col customWidth="1" min="5" max="5" width="28.7109375"/>
-    <col customWidth="1" min="6" max="7" width="25.00390625"/>
+    <col customWidth="1" min="3" max="6" width="18.421875"/>
+    <col customWidth="1" min="7" max="7" width="28.7109375"/>
+    <col customWidth="1" min="8" max="10" width="25.00390625"/>
   </cols>
   <sheetData>
+    <row r="1" ht="14.25">
+      <c r="F1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
     <row r="2" ht="16.5">
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -5636,10 +5851,19 @@
         <v>7</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>6</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -5653,14 +5877,24 @@
         <v>1</v>
       </c>
       <c r="E3" s="20">
-        <f t="shared" ref="E3:E9" si="6">ABS(C3-D3)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="20">
+        <f>ABS(C3-D3)</f>
         <v>0</v>
       </c>
-      <c r="F3" s="21">
+      <c r="G3" s="20">
+        <f>ABS(C3-E3)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="21">
         <v>41980</v>
       </c>
-      <c r="G3" s="21">
+      <c r="I3" s="21">
         <v>41980</v>
+      </c>
+      <c r="J3" s="21">
+        <v>42047</v>
       </c>
     </row>
     <row r="4">
@@ -5668,22 +5902,33 @@
         <v>2</v>
       </c>
       <c r="C4" s="20">
-        <f t="shared" ref="C4:C9" si="7">$F$3/F4</f>
+        <f>$H$3/H4</f>
         <v>1.5994818258020269</v>
       </c>
       <c r="D4" s="20">
-        <f t="shared" ref="D4:D9" si="8">$G$3/G4</f>
+        <f>$I$3/I4</f>
         <v>1.5994818258020269</v>
       </c>
       <c r="E4" s="20">
-        <f t="shared" si="6"/>
+        <f>$J$3/J4</f>
+        <v>2.0002378573807147</v>
+      </c>
+      <c r="F4" s="20">
+        <f>ABS(C4-D4)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="21">
+      <c r="G4" s="20">
+        <f>ABS(C4-E4)</f>
+        <v>0.40075603157868778</v>
+      </c>
+      <c r="H4" s="21">
         <v>26246</v>
       </c>
-      <c r="G4" s="21">
+      <c r="I4" s="21">
         <v>26246</v>
+      </c>
+      <c r="J4" s="21">
+        <v>21021</v>
       </c>
     </row>
     <row r="5">
@@ -5691,22 +5936,33 @@
         <v>3</v>
       </c>
       <c r="C5" s="20">
-        <f t="shared" si="7"/>
+        <f>$H$3/H5</f>
         <v>2.0001905850962456</v>
       </c>
       <c r="D5" s="20">
-        <f t="shared" si="8"/>
+        <f>$I$3/I5</f>
         <v>2.0001905850962456</v>
       </c>
       <c r="E5" s="20">
-        <f t="shared" si="6"/>
+        <f>$J$3/J5</f>
+        <v>2.0002378573807147</v>
+      </c>
+      <c r="F5" s="20">
+        <f>ABS(C5-D5)</f>
         <v>0</v>
       </c>
-      <c r="F5" s="21">
+      <c r="G5" s="20">
+        <f>ABS(C5-E5)</f>
+        <v>4.7272284469102033e-05</v>
+      </c>
+      <c r="H5" s="21">
         <v>20988</v>
       </c>
-      <c r="G5" s="21">
+      <c r="I5" s="21">
         <v>20988</v>
+      </c>
+      <c r="J5" s="21">
+        <v>21021</v>
       </c>
     </row>
     <row r="6">
@@ -5714,22 +5970,33 @@
         <v>4</v>
       </c>
       <c r="C6" s="20">
-        <f t="shared" si="7"/>
+        <f>$H$3/H6</f>
         <v>2.1808925138968256</v>
       </c>
       <c r="D6" s="20">
-        <f t="shared" si="8"/>
+        <f>$I$3/I6</f>
         <v>2.1808925138968256</v>
       </c>
       <c r="E6" s="20">
-        <f t="shared" si="6"/>
+        <f>$J$3/J6</f>
+        <v>2.666603247082699</v>
+      </c>
+      <c r="F6" s="20">
+        <f>ABS(C6-D6)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="21">
+      <c r="G6" s="20">
+        <f>ABS(C6-E6)</f>
+        <v>0.48571073318587343</v>
+      </c>
+      <c r="H6" s="21">
         <v>19249</v>
       </c>
-      <c r="G6" s="21">
+      <c r="I6" s="21">
         <v>19249</v>
+      </c>
+      <c r="J6" s="21">
+        <v>15768</v>
       </c>
     </row>
     <row r="7">
@@ -5737,22 +6004,33 @@
         <v>5</v>
       </c>
       <c r="C7" s="20">
-        <f t="shared" si="7"/>
+        <f>$H$3/H7</f>
         <v>2.4989582713256739</v>
       </c>
       <c r="D7" s="20">
-        <f t="shared" si="8"/>
+        <f>$I$3/I7</f>
         <v>2.4989582713256739</v>
       </c>
       <c r="E7" s="20">
-        <f t="shared" si="6"/>
+        <f>$J$3/J7</f>
+        <v>2.5004162702188393</v>
+      </c>
+      <c r="F7" s="20">
+        <f>ABS(C7-D7)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="21">
+      <c r="G7" s="20">
+        <f>ABS(C7-E7)</f>
+        <v>0.0014579988931653354</v>
+      </c>
+      <c r="H7" s="21">
         <v>16799</v>
       </c>
-      <c r="G7" s="21">
+      <c r="I7" s="21">
         <v>16799</v>
+      </c>
+      <c r="J7" s="21">
+        <v>16816</v>
       </c>
     </row>
     <row r="8">
@@ -5760,22 +6038,33 @@
         <v>6</v>
       </c>
       <c r="C8" s="20">
-        <f t="shared" si="7"/>
+        <f>$H$3/H8</f>
         <v>2.5242017918345261</v>
       </c>
       <c r="D8" s="20">
-        <f t="shared" si="8"/>
+        <f>$I$3/I8</f>
         <v>2.5242017918345261</v>
       </c>
       <c r="E8" s="20">
-        <f t="shared" si="6"/>
+        <f>$J$3/J8</f>
+        <v>3.0005708984514379</v>
+      </c>
+      <c r="F8" s="20">
+        <f>ABS(C8-D8)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="21">
+      <c r="G8" s="20">
+        <f>ABS(C8-E8)</f>
+        <v>0.47636910661691179</v>
+      </c>
+      <c r="H8" s="21">
         <v>16631</v>
       </c>
-      <c r="G8" s="21">
+      <c r="I8" s="21">
         <v>16631</v>
+      </c>
+      <c r="J8" s="21">
+        <v>14013</v>
       </c>
     </row>
     <row r="9">
@@ -5783,22 +6072,33 @@
         <v>7</v>
       </c>
       <c r="C9" s="20">
-        <f t="shared" si="7"/>
+        <f>$H$3/H9</f>
         <v>2.7962432558449346</v>
       </c>
       <c r="D9" s="20">
-        <f t="shared" si="8"/>
+        <f>$I$3/I9</f>
         <v>2.7962432558449346</v>
       </c>
       <c r="E9" s="20">
-        <f t="shared" si="6"/>
+        <f>$J$3/J9</f>
+        <v>2.8005195151192219</v>
+      </c>
+      <c r="F9" s="20">
+        <f>ABS(C9-D9)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="21">
+      <c r="G9" s="20">
+        <f>ABS(C9-E9)</f>
+        <v>0.0042762592742873196</v>
+      </c>
+      <c r="H9" s="21">
         <v>15013</v>
       </c>
-      <c r="G9" s="21">
+      <c r="I9" s="21">
         <v>15013</v>
+      </c>
+      <c r="J9" s="21">
+        <v>15014</v>
       </c>
     </row>
     <row r="10">
@@ -5806,22 +6106,33 @@
         <v>8</v>
       </c>
       <c r="C10" s="20">
-        <f t="shared" ref="C10:C66" si="9">$F$3/F10</f>
+        <f>$H$3/H10</f>
         <v>2.7544124401286005</v>
       </c>
       <c r="D10" s="20">
-        <f t="shared" ref="D10:D66" si="10">$G$3/G10</f>
+        <f>$I$3/I10</f>
         <v>2.7544124401286005</v>
       </c>
       <c r="E10" s="20">
-        <f t="shared" ref="E10:E66" si="11">ABS(C10-D10)</f>
+        <f>$J$3/J10</f>
+        <v>3.1991934870273151</v>
+      </c>
+      <c r="F10" s="20">
+        <f>ABS(C10-D10)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="21">
+      <c r="G10" s="20">
+        <f>ABS(C10-E10)</f>
+        <v>0.44478104689871456</v>
+      </c>
+      <c r="H10" s="21">
         <v>15241</v>
       </c>
-      <c r="G10" s="21">
+      <c r="I10" s="21">
         <v>15241</v>
+      </c>
+      <c r="J10" s="21">
+        <v>13143</v>
       </c>
     </row>
     <row r="11">
@@ -5829,21 +6140,32 @@
         <v>9</v>
       </c>
       <c r="C11" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H11</f>
         <v>2.9938667807730708</v>
       </c>
       <c r="D11" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I11</f>
         <v>2.9938667807730708</v>
       </c>
       <c r="E11" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J11</f>
+        <v>2.9986449864498645</v>
+      </c>
+      <c r="F11" s="20">
+        <f>ABS(C11-D11)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="21">
+      <c r="G11" s="20">
+        <f>ABS(C11-E11)</f>
+        <v>0.0047782056767937675</v>
+      </c>
+      <c r="H11" s="21">
         <v>14022</v>
       </c>
-      <c r="G11" s="21">
+      <c r="I11" s="21">
+        <v>14022</v>
+      </c>
+      <c r="J11" s="21">
         <v>14022</v>
       </c>
     </row>
@@ -5852,22 +6174,33 @@
         <v>10</v>
       </c>
       <c r="C12" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H12</f>
         <v>2.9205509948518156</v>
       </c>
       <c r="D12" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I12</f>
         <v>2.9205509948518156</v>
       </c>
       <c r="E12" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J12</f>
+        <v>3.3299279322087592</v>
+      </c>
+      <c r="F12" s="20">
+        <f>ABS(C12-D12)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="21">
+      <c r="G12" s="20">
+        <f>ABS(C12-E12)</f>
+        <v>0.40937693735694358</v>
+      </c>
+      <c r="H12" s="21">
         <v>14374</v>
       </c>
-      <c r="G12" s="21">
+      <c r="I12" s="21">
         <v>14374</v>
+      </c>
+      <c r="J12" s="21">
+        <v>12627</v>
       </c>
     </row>
     <row r="13">
@@ -5875,22 +6208,33 @@
         <v>11</v>
       </c>
       <c r="C13" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H13</f>
         <v>3.1335373591102487</v>
       </c>
       <c r="D13" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I13</f>
         <v>3.1335373591102487</v>
       </c>
       <c r="E13" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J13</f>
+        <v>3.1399447390038087</v>
+      </c>
+      <c r="F13" s="20">
+        <f>ABS(C13-D13)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="21">
+      <c r="G13" s="20">
+        <f>ABS(C13-E13)</f>
+        <v>0.0064073798935599946</v>
+      </c>
+      <c r="H13" s="21">
         <v>13397</v>
       </c>
-      <c r="G13" s="21">
+      <c r="I13" s="21">
         <v>13397</v>
+      </c>
+      <c r="J13" s="21">
+        <v>13391</v>
       </c>
     </row>
     <row r="14">
@@ -5898,22 +6242,33 @@
         <v>12</v>
       </c>
       <c r="C14" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H14</f>
         <v>3.0448973670849351</v>
       </c>
       <c r="D14" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I14</f>
         <v>3.0448973670849351</v>
       </c>
       <c r="E14" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J14</f>
+        <v>3.4220721087328072</v>
+      </c>
+      <c r="F14" s="20">
+        <f>ABS(C14-D14)</f>
         <v>0</v>
       </c>
-      <c r="F14" s="21">
+      <c r="G14" s="20">
+        <f>ABS(C14-E14)</f>
+        <v>0.37717474164787212</v>
+      </c>
+      <c r="H14" s="21">
         <v>13787</v>
       </c>
-      <c r="G14" s="21">
+      <c r="I14" s="21">
         <v>13787</v>
+      </c>
+      <c r="J14" s="21">
+        <v>12287</v>
       </c>
     </row>
     <row r="15">
@@ -5921,22 +6276,33 @@
         <v>13</v>
       </c>
       <c r="C15" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H15</f>
         <v>3.23769859632886</v>
       </c>
       <c r="D15" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I15</f>
         <v>3.23769859632886</v>
       </c>
       <c r="E15" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J15</f>
+        <v>3.2446176402500191</v>
+      </c>
+      <c r="F15" s="20">
+        <f>ABS(C15-D15)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="21">
+      <c r="G15" s="20">
+        <f>ABS(C15-E15)</f>
+        <v>0.0069190439211590515</v>
+      </c>
+      <c r="H15" s="21">
         <v>12966</v>
       </c>
-      <c r="G15" s="21">
+      <c r="I15" s="21">
         <v>12966</v>
+      </c>
+      <c r="J15" s="21">
+        <v>12959</v>
       </c>
     </row>
     <row r="16">
@@ -5944,22 +6310,33 @@
         <v>14</v>
       </c>
       <c r="C16" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H16</f>
         <v>3.1419803906893198</v>
       </c>
       <c r="D16" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I16</f>
         <v>3.1419803906893198</v>
       </c>
       <c r="E16" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J16</f>
+        <v>3.4896671922981159</v>
+      </c>
+      <c r="F16" s="20">
+        <f>ABS(C16-D16)</f>
         <v>0</v>
       </c>
-      <c r="F16" s="21">
+      <c r="G16" s="20">
+        <f>ABS(C16-E16)</f>
+        <v>0.34768680160879617</v>
+      </c>
+      <c r="H16" s="21">
         <v>13361</v>
       </c>
-      <c r="G16" s="21">
+      <c r="I16" s="21">
         <v>13361</v>
+      </c>
+      <c r="J16" s="21">
+        <v>12049</v>
       </c>
     </row>
     <row r="17">
@@ -5967,22 +6344,33 @@
         <v>15</v>
       </c>
       <c r="C17" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H17</f>
         <v>3.3172659028052154</v>
       </c>
       <c r="D17" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I17</f>
         <v>3.3172659028052154</v>
       </c>
       <c r="E17" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J17</f>
+        <v>3.3241362953593168</v>
+      </c>
+      <c r="F17" s="20">
+        <f>ABS(C17-D17)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="21">
+      <c r="G17" s="20">
+        <f>ABS(C17-E17)</f>
+        <v>0.0068703925541013788</v>
+      </c>
+      <c r="H17" s="21">
         <v>12655</v>
       </c>
-      <c r="G17" s="21">
+      <c r="I17" s="21">
         <v>12655</v>
+      </c>
+      <c r="J17" s="21">
+        <v>12649</v>
       </c>
     </row>
     <row r="18">
@@ -5990,22 +6378,33 @@
         <v>16</v>
       </c>
       <c r="C18" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H18</f>
         <v>3.2198189906427368</v>
       </c>
       <c r="D18" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I18</f>
         <v>3.2198189906427368</v>
       </c>
       <c r="E18" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J18</f>
+        <v>3.5416947439353099</v>
+      </c>
+      <c r="F18" s="20">
+        <f>ABS(C18-D18)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="21">
+      <c r="G18" s="20">
+        <f>ABS(C18-E18)</f>
+        <v>0.32187575329257312</v>
+      </c>
+      <c r="H18" s="21">
         <v>13038</v>
       </c>
-      <c r="G18" s="21">
+      <c r="I18" s="21">
         <v>13038</v>
+      </c>
+      <c r="J18" s="21">
+        <v>11872</v>
       </c>
     </row>
     <row r="19">
@@ -6013,22 +6412,33 @@
         <v>17</v>
       </c>
       <c r="C19" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H19</f>
         <v>3.3794880051521492</v>
       </c>
       <c r="D19" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I19</f>
         <v>3.3794880051521492</v>
       </c>
       <c r="E19" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J19</f>
+        <v>3.3862446645727631</v>
+      </c>
+      <c r="F19" s="20">
+        <f>ABS(C19-D19)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="21">
+      <c r="G19" s="20">
+        <f>ABS(C19-E19)</f>
+        <v>0.0067566594206138753</v>
+      </c>
+      <c r="H19" s="21">
         <v>12422</v>
       </c>
-      <c r="G19" s="21">
+      <c r="I19" s="21">
         <v>12422</v>
+      </c>
+      <c r="J19" s="21">
+        <v>12417</v>
       </c>
     </row>
     <row r="20">
@@ -6036,22 +6446,33 @@
         <v>18</v>
       </c>
       <c r="C20" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H20</f>
         <v>3.2853341681014245</v>
       </c>
       <c r="D20" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I20</f>
         <v>3.2853341681014245</v>
       </c>
       <c r="E20" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J20</f>
+        <v>3.5815161839863712</v>
+      </c>
+      <c r="F20" s="20">
+        <f>ABS(C20-D20)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="21">
+      <c r="G20" s="20">
+        <f>ABS(C20-E20)</f>
+        <v>0.29618201588494664</v>
+      </c>
+      <c r="H20" s="21">
         <v>12778</v>
       </c>
-      <c r="G20" s="21">
+      <c r="I20" s="21">
         <v>12778</v>
+      </c>
+      <c r="J20" s="21">
+        <v>11740</v>
       </c>
     </row>
     <row r="21">
@@ -6059,22 +6480,33 @@
         <v>19</v>
       </c>
       <c r="C21" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H21</f>
         <v>3.4288981458792778</v>
       </c>
       <c r="D21" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I21</f>
         <v>3.4288981458792778</v>
       </c>
       <c r="E21" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J21</f>
+        <v>3.4374591236102026</v>
+      </c>
+      <c r="F21" s="20">
+        <f>ABS(C21-D21)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="21">
+      <c r="G21" s="20">
+        <f>ABS(C21-E21)</f>
+        <v>0.0085609777309247903</v>
+      </c>
+      <c r="H21" s="21">
         <v>12243</v>
       </c>
-      <c r="G21" s="21">
+      <c r="I21" s="21">
         <v>12243</v>
+      </c>
+      <c r="J21" s="21">
+        <v>12232</v>
       </c>
     </row>
     <row r="22">
@@ -6082,22 +6514,33 @@
         <v>20</v>
       </c>
       <c r="C22" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H22</f>
         <v>3.3346572404480104</v>
       </c>
       <c r="D22" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I22</f>
         <v>3.3346572404480104</v>
       </c>
       <c r="E22" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J22</f>
+        <v>3.6132164647245855</v>
+      </c>
+      <c r="F22" s="20">
+        <f>ABS(C22-D22)</f>
         <v>0</v>
       </c>
-      <c r="F22" s="21">
+      <c r="G22" s="20">
+        <f>ABS(C22-E22)</f>
+        <v>0.27855922427657509</v>
+      </c>
+      <c r="H22" s="21">
         <v>12589</v>
       </c>
-      <c r="G22" s="21">
+      <c r="I22" s="21">
         <v>12589</v>
+      </c>
+      <c r="J22" s="21">
+        <v>11637</v>
       </c>
     </row>
     <row r="23">
@@ -6105,22 +6548,33 @@
         <v>21</v>
       </c>
       <c r="C23" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H23</f>
         <v>3.4705687830687832</v>
       </c>
       <c r="D23" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I23</f>
         <v>3.4705687830687832</v>
       </c>
       <c r="E23" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J23</f>
+        <v>3.4810000827883103</v>
+      </c>
+      <c r="F23" s="20">
+        <f>ABS(C23-D23)</f>
         <v>0</v>
       </c>
-      <c r="F23" s="21">
+      <c r="G23" s="20">
+        <f>ABS(C23-E23)</f>
+        <v>0.010431299719527054</v>
+      </c>
+      <c r="H23" s="21">
         <v>12096</v>
       </c>
-      <c r="G23" s="21">
+      <c r="I23" s="21">
         <v>12096</v>
+      </c>
+      <c r="J23" s="21">
+        <v>12079</v>
       </c>
     </row>
     <row r="24">
@@ -6128,22 +6582,33 @@
         <v>22</v>
       </c>
       <c r="C24" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H24</f>
         <v>3.3797600837291681</v>
       </c>
       <c r="D24" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I24</f>
         <v>3.3797600837291681</v>
       </c>
       <c r="E24" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J24</f>
+        <v>3.6394875789838137</v>
+      </c>
+      <c r="F24" s="20">
+        <f>ABS(C24-D24)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="21">
+      <c r="G24" s="20">
+        <f>ABS(C24-E24)</f>
+        <v>0.25972749525464556</v>
+      </c>
+      <c r="H24" s="21">
         <v>12421</v>
       </c>
-      <c r="G24" s="21">
+      <c r="I24" s="21">
         <v>12421</v>
+      </c>
+      <c r="J24" s="21">
+        <v>11553</v>
       </c>
     </row>
     <row r="25">
@@ -6151,22 +6616,33 @@
         <v>23</v>
       </c>
       <c r="C25" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H25</f>
         <v>3.5050513484178007</v>
       </c>
       <c r="D25" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I25</f>
         <v>3.5050513484178007</v>
       </c>
       <c r="E25" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J25</f>
+        <v>3.5147538242915655</v>
+      </c>
+      <c r="F25" s="20">
+        <f>ABS(C25-D25)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="21">
+      <c r="G25" s="20">
+        <f>ABS(C25-E25)</f>
+        <v>0.0097024758737647154</v>
+      </c>
+      <c r="H25" s="21">
         <v>11977</v>
       </c>
-      <c r="G25" s="21">
+      <c r="I25" s="21">
         <v>11977</v>
+      </c>
+      <c r="J25" s="21">
+        <v>11963</v>
       </c>
     </row>
     <row r="26">
@@ -6174,22 +6650,33 @@
         <v>24</v>
       </c>
       <c r="C26" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H26</f>
         <v>3.4168972814585707</v>
       </c>
       <c r="D26" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I26</f>
         <v>3.4168972814585707</v>
       </c>
       <c r="E26" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J26</f>
+        <v>3.6610361340879409</v>
+      </c>
+      <c r="F26" s="20">
+        <f>ABS(C26-D26)</f>
         <v>0</v>
       </c>
-      <c r="F26" s="21">
+      <c r="G26" s="20">
+        <f>ABS(C26-E26)</f>
+        <v>0.24413885262937018</v>
+      </c>
+      <c r="H26" s="21">
         <v>12286</v>
       </c>
-      <c r="G26" s="21">
+      <c r="I26" s="21">
         <v>12286</v>
+      </c>
+      <c r="J26" s="21">
+        <v>11485</v>
       </c>
     </row>
     <row r="27">
@@ -6197,22 +6684,33 @@
         <v>25</v>
       </c>
       <c r="C27" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H27</f>
         <v>3.5345625999831607</v>
       </c>
       <c r="D27" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I27</f>
         <v>3.5345625999831607</v>
       </c>
       <c r="E27" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J27</f>
+        <v>3.5425899401803016</v>
+      </c>
+      <c r="F27" s="20">
+        <f>ABS(C27-D27)</f>
         <v>0</v>
       </c>
-      <c r="F27" s="21">
+      <c r="G27" s="20">
+        <f>ABS(C27-E27)</f>
+        <v>0.0080273401971409086</v>
+      </c>
+      <c r="H27" s="21">
         <v>11877</v>
       </c>
-      <c r="G27" s="21">
+      <c r="I27" s="21">
         <v>11877</v>
+      </c>
+      <c r="J27" s="21">
+        <v>11869</v>
       </c>
     </row>
     <row r="28">
@@ -6220,22 +6718,33 @@
         <v>26</v>
       </c>
       <c r="C28" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H28</f>
         <v>3.4469168240413826</v>
       </c>
       <c r="D28" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I28</f>
         <v>3.4469168240413826</v>
       </c>
       <c r="E28" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J28</f>
+        <v>3.678652668416448</v>
+      </c>
+      <c r="F28" s="20">
+        <f>ABS(C28-D28)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="22">
+      <c r="G28" s="20">
+        <f>ABS(C28-E28)</f>
+        <v>0.23173584437506545</v>
+      </c>
+      <c r="H28" s="22">
         <v>12179</v>
       </c>
-      <c r="G28" s="22">
+      <c r="I28" s="22">
         <v>12179</v>
+      </c>
+      <c r="J28" s="22">
+        <v>11430</v>
       </c>
     </row>
     <row r="29">
@@ -6243,22 +6752,33 @@
         <v>27</v>
       </c>
       <c r="C29" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H29</f>
         <v>3.5558190750465863</v>
       </c>
       <c r="D29" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I29</f>
         <v>3.5558190750465863</v>
       </c>
       <c r="E29" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J29</f>
+        <v>3.5708704883227176</v>
+      </c>
+      <c r="F29" s="20">
+        <f>ABS(C29-D29)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="22">
+      <c r="G29" s="20">
+        <f>ABS(C29-E29)</f>
+        <v>0.015051413276131242</v>
+      </c>
+      <c r="H29" s="22">
         <v>11806</v>
       </c>
-      <c r="G29" s="22">
+      <c r="I29" s="22">
         <v>11806</v>
+      </c>
+      <c r="J29" s="22">
+        <v>11775</v>
       </c>
     </row>
     <row r="30">
@@ -6266,22 +6786,33 @@
         <v>28</v>
       </c>
       <c r="C30" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H30</f>
         <v>3.4760288151030885</v>
       </c>
       <c r="D30" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I30</f>
         <v>3.476316661146075</v>
       </c>
       <c r="E30" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J30</f>
+        <v>3.6902755836405126</v>
+      </c>
+      <c r="F30" s="20">
+        <f>ABS(C30-D30)</f>
         <v>0.00028784604298648375</v>
       </c>
-      <c r="F30" s="22">
+      <c r="G30" s="20">
+        <f>ABS(C30-E30)</f>
+        <v>0.21424676853742408</v>
+      </c>
+      <c r="H30" s="22">
         <v>12077</v>
       </c>
-      <c r="G30" s="22">
+      <c r="I30" s="22">
         <v>12076</v>
+      </c>
+      <c r="J30" s="22">
+        <v>11394</v>
       </c>
     </row>
     <row r="31">
@@ -6289,22 +6820,33 @@
         <v>29</v>
       </c>
       <c r="C31" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H31</f>
         <v>3.5800784581272387</v>
       </c>
       <c r="D31" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I31</f>
         <v>3.5800784581272387</v>
       </c>
       <c r="E31" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J31</f>
+        <v>3.5897720481516262</v>
+      </c>
+      <c r="F31" s="20">
+        <f>ABS(C31-D31)</f>
         <v>0</v>
       </c>
-      <c r="F31" s="22">
+      <c r="G31" s="20">
+        <f>ABS(C31-E31)</f>
+        <v>0.0096935900243875217</v>
+      </c>
+      <c r="H31" s="22">
         <v>11726</v>
       </c>
-      <c r="G31" s="22">
+      <c r="I31" s="22">
         <v>11726</v>
+      </c>
+      <c r="J31" s="22">
+        <v>11713</v>
       </c>
     </row>
     <row r="32">
@@ -6312,22 +6854,33 @@
         <v>30</v>
       </c>
       <c r="C32" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H32</f>
         <v>3.501835168501835</v>
       </c>
       <c r="D32" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I32</f>
         <v>3.501835168501835</v>
       </c>
       <c r="E32" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J32</f>
+        <v>3.7039288231148695</v>
+      </c>
+      <c r="F32" s="20">
+        <f>ABS(C32-D32)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="22">
+      <c r="G32" s="20">
+        <f>ABS(C32-E32)</f>
+        <v>0.20209365461303452</v>
+      </c>
+      <c r="H32" s="22">
         <v>11988</v>
       </c>
-      <c r="G32" s="22">
+      <c r="I32" s="22">
         <v>11988</v>
+      </c>
+      <c r="J32" s="22">
+        <v>11352</v>
       </c>
     </row>
     <row r="33">
@@ -6335,46 +6888,68 @@
         <v>31</v>
       </c>
       <c r="C33" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H33</f>
         <v>3.5960253554908341</v>
       </c>
       <c r="D33" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I33</f>
         <v>3.5978745286253</v>
       </c>
       <c r="E33" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J33</f>
+        <v>3.6088747746974508</v>
+      </c>
+      <c r="F33" s="20">
+        <f>ABS(C33-D33)</f>
         <v>0.0018491731344658646</v>
       </c>
-      <c r="F33" s="22">
+      <c r="G33" s="20">
+        <f>ABS(C33-E33)</f>
+        <v>0.012849419206616641</v>
+      </c>
+      <c r="H33" s="22">
         <v>11674</v>
       </c>
-      <c r="G33" s="22">
+      <c r="I33" s="22">
         <v>11668</v>
       </c>
-      <c r="L33" s="23"/>
+      <c r="J33" s="22">
+        <v>11651</v>
+      </c>
+      <c r="O33" s="23"/>
     </row>
     <row r="34">
       <c r="B34" s="7">
         <v>32</v>
       </c>
       <c r="C34" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H34</f>
         <v>3.5221075593590068</v>
       </c>
       <c r="D34" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I34</f>
         <v>3.5218120805369129</v>
       </c>
       <c r="E34" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J34</f>
+        <v>3.7166976045257667</v>
+      </c>
+      <c r="F34" s="20">
+        <f>ABS(C34-D34)</f>
         <v>0.00029547882209390863</v>
       </c>
-      <c r="F34" s="22">
+      <c r="G34" s="20">
+        <f>ABS(C34-E34)</f>
+        <v>0.19459004516675993</v>
+      </c>
+      <c r="H34" s="22">
         <v>11919</v>
       </c>
-      <c r="G34" s="22">
+      <c r="I34" s="22">
         <v>11920</v>
+      </c>
+      <c r="J34" s="22">
+        <v>11313</v>
       </c>
     </row>
     <row r="35" ht="14.25">
@@ -6382,22 +6957,33 @@
         <v>33</v>
       </c>
       <c r="C35" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H35</f>
         <v>3.6174062903920725</v>
       </c>
       <c r="D35" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I35</f>
         <v>3.6174062903920725</v>
       </c>
       <c r="E35" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J35</f>
+        <v>3.623804188571921</v>
+      </c>
+      <c r="F35" s="20">
+        <f>ABS(C35-D35)</f>
         <v>0</v>
       </c>
-      <c r="F35" s="21">
+      <c r="G35" s="20">
+        <f>ABS(C35-E35)</f>
+        <v>0.0063978981798484824</v>
+      </c>
+      <c r="H35" s="21">
         <v>11605</v>
       </c>
-      <c r="G35" s="21">
+      <c r="I35" s="21">
         <v>11605</v>
+      </c>
+      <c r="J35" s="21">
+        <v>11603</v>
       </c>
     </row>
     <row r="36" ht="14.25">
@@ -6405,22 +6991,33 @@
         <v>34</v>
       </c>
       <c r="C36" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H36</f>
         <v>3.5423171040418531</v>
       </c>
       <c r="D36" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I36</f>
         <v>3.5396290050590218</v>
       </c>
       <c r="E36" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J36</f>
+        <v>3.7305474225889452</v>
+      </c>
+      <c r="F36" s="20">
+        <f>ABS(C36-D36)</f>
         <v>0.0026880989828312885</v>
       </c>
-      <c r="F36" s="21">
+      <c r="G36" s="20">
+        <f>ABS(C36-E36)</f>
+        <v>0.18823031854709216</v>
+      </c>
+      <c r="H36" s="21">
         <v>11851</v>
       </c>
-      <c r="G36" s="21">
+      <c r="I36" s="21">
         <v>11860</v>
+      </c>
+      <c r="J36" s="21">
+        <v>11271</v>
       </c>
     </row>
     <row r="37" ht="14.25">
@@ -6428,22 +7025,33 @@
         <v>35</v>
       </c>
       <c r="C37" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H37</f>
         <v>3.6227131515360718</v>
       </c>
       <c r="D37" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I37</f>
         <v>3.6233385119972379</v>
       </c>
       <c r="E37" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J37</f>
+        <v>3.638227913818465</v>
+      </c>
+      <c r="F37" s="20">
+        <f>ABS(C37-D37)</f>
         <v>0.00062536046116612454</v>
       </c>
-      <c r="F37" s="21">
+      <c r="G37" s="20">
+        <f>ABS(C37-E37)</f>
+        <v>0.015514762282393235</v>
+      </c>
+      <c r="H37" s="21">
         <v>11588</v>
       </c>
-      <c r="G37" s="21">
+      <c r="I37" s="21">
         <v>11586</v>
+      </c>
+      <c r="J37" s="21">
+        <v>11557</v>
       </c>
     </row>
     <row r="38" ht="14.25">
@@ -6451,22 +7059,33 @@
         <v>36</v>
       </c>
       <c r="C38" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H38</f>
         <v>3.5558190750465863</v>
       </c>
       <c r="D38" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I38</f>
         <v>3.557627118644068</v>
       </c>
       <c r="E38" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J38</f>
+        <v>3.7331971943531919</v>
+      </c>
+      <c r="F38" s="20">
+        <f>ABS(C38-D38)</f>
         <v>0.0018080435974816567</v>
       </c>
-      <c r="F38" s="21">
+      <c r="G38" s="20">
+        <f>ABS(C38-E38)</f>
+        <v>0.17737811930660552</v>
+      </c>
+      <c r="H38" s="21">
         <v>11806</v>
       </c>
-      <c r="G38" s="21">
+      <c r="I38" s="21">
         <v>11800</v>
+      </c>
+      <c r="J38" s="21">
+        <v>11263</v>
       </c>
     </row>
     <row r="39" ht="14.25">
@@ -6474,22 +7093,33 @@
         <v>37</v>
       </c>
       <c r="C39" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H39</f>
         <v>3.6380968888118557</v>
       </c>
       <c r="D39" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I39</f>
         <v>3.6384122031547927</v>
       </c>
       <c r="E39" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J39</f>
+        <v>3.6502300546922477</v>
+      </c>
+      <c r="F39" s="20">
+        <f>ABS(C39-D39)</f>
         <v>0.00031531434293707861</v>
       </c>
-      <c r="F39" s="21">
+      <c r="G39" s="20">
+        <f>ABS(C39-E39)</f>
+        <v>0.012133165880392038</v>
+      </c>
+      <c r="H39" s="21">
         <v>11539</v>
       </c>
-      <c r="G39" s="21">
+      <c r="I39" s="21">
         <v>11538</v>
+      </c>
+      <c r="J39" s="21">
+        <v>11519</v>
       </c>
     </row>
     <row r="40" ht="14.25">
@@ -6497,22 +7127,33 @@
         <v>38</v>
       </c>
       <c r="C40" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H40</f>
         <v>3.5724619181346267</v>
       </c>
       <c r="D40" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I40</f>
         <v>3.5730700485147673</v>
       </c>
       <c r="E40" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J40</f>
+        <v>3.7388404766139072</v>
+      </c>
+      <c r="F40" s="20">
+        <f>ABS(C40-D40)</f>
         <v>0.0006081303801406257</v>
       </c>
-      <c r="F40" s="21">
+      <c r="G40" s="20">
+        <f>ABS(C40-E40)</f>
+        <v>0.16637855847928051</v>
+      </c>
+      <c r="H40" s="21">
         <v>11751</v>
       </c>
-      <c r="G40" s="21">
+      <c r="I40" s="21">
         <v>11749</v>
+      </c>
+      <c r="J40" s="21">
+        <v>11246</v>
       </c>
     </row>
     <row r="41" ht="14.25">
@@ -6520,22 +7161,33 @@
         <v>39</v>
       </c>
       <c r="C41" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H41</f>
         <v>3.6501173810972958</v>
       </c>
       <c r="D41" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I41</f>
         <v>3.6447299878451118</v>
       </c>
       <c r="E41" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J41</f>
+        <v>3.6578512396694216</v>
+      </c>
+      <c r="F41" s="20">
+        <f>ABS(C41-D41)</f>
         <v>0.0053873932521839585</v>
       </c>
-      <c r="F41" s="21">
+      <c r="G41" s="20">
+        <f>ABS(C41-E41)</f>
+        <v>0.0077338585721258291</v>
+      </c>
+      <c r="H41" s="21">
         <v>11501</v>
       </c>
-      <c r="G41" s="21">
+      <c r="I41" s="21">
         <v>11518</v>
+      </c>
+      <c r="J41" s="21">
+        <v>11495</v>
       </c>
     </row>
     <row r="42" ht="14.25">
@@ -6543,22 +7195,33 @@
         <v>40</v>
       </c>
       <c r="C42" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H42</f>
         <v>3.5809946259489891</v>
       </c>
       <c r="D42" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I42</f>
         <v>3.5828283690364429</v>
       </c>
       <c r="E42" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J42</f>
+        <v>3.7445008460236888</v>
+      </c>
+      <c r="F42" s="20">
+        <f>ABS(C42-D42)</f>
         <v>0.0018337430874537652</v>
       </c>
-      <c r="F42" s="21">
+      <c r="G42" s="20">
+        <f>ABS(C42-E42)</f>
+        <v>0.16350622007469973</v>
+      </c>
+      <c r="H42" s="21">
         <v>11723</v>
       </c>
-      <c r="G42" s="21">
+      <c r="I42" s="21">
         <v>11717</v>
+      </c>
+      <c r="J42" s="21">
+        <v>11229</v>
       </c>
     </row>
     <row r="43" ht="14.25">
@@ -6566,22 +7229,33 @@
         <v>41</v>
       </c>
       <c r="C43" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H43</f>
         <v>3.6571129889363183</v>
       </c>
       <c r="D43" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I43</f>
         <v>3.6567944250871078</v>
       </c>
       <c r="E43" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J43</f>
+        <v>3.6687025564959428</v>
+      </c>
+      <c r="F43" s="20">
+        <f>ABS(C43-D43)</f>
         <v>0.00031856384921047365</v>
       </c>
-      <c r="F43" s="21">
+      <c r="G43" s="20">
+        <f>ABS(C43-E43)</f>
+        <v>0.011589567559624481</v>
+      </c>
+      <c r="H43" s="21">
         <v>11479</v>
       </c>
-      <c r="G43" s="21">
+      <c r="I43" s="21">
         <v>11480</v>
+      </c>
+      <c r="J43" s="21">
+        <v>11461</v>
       </c>
     </row>
     <row r="44" ht="14.25">
@@ -6589,22 +7263,33 @@
         <v>42</v>
       </c>
       <c r="C44" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H44</f>
         <v>3.5923327058018142</v>
       </c>
       <c r="D44" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I44</f>
         <v>3.5923327058018142</v>
       </c>
       <c r="E44" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J44</f>
+        <v>3.7491752117699511</v>
+      </c>
+      <c r="F44" s="20">
+        <f>ABS(C44-D44)</f>
         <v>0</v>
       </c>
-      <c r="F44" s="21">
+      <c r="G44" s="20">
+        <f>ABS(C44-E44)</f>
+        <v>0.15684250596813687</v>
+      </c>
+      <c r="H44" s="21">
         <v>11686</v>
       </c>
-      <c r="G44" s="21">
+      <c r="I44" s="21">
         <v>11686</v>
+      </c>
+      <c r="J44" s="21">
+        <v>11215</v>
       </c>
     </row>
     <row r="45" ht="14.25">
@@ -6612,22 +7297,33 @@
         <v>43</v>
       </c>
       <c r="C45" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H45</f>
         <v>3.6634959420542805</v>
       </c>
       <c r="D45" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I45</f>
         <v>3.6634959420542805</v>
       </c>
       <c r="E45" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J45</f>
+        <v>3.6764011541488153</v>
+      </c>
+      <c r="F45" s="20">
+        <f>ABS(C45-D45)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="21">
+      <c r="G45" s="20">
+        <f>ABS(C45-E45)</f>
+        <v>0.012905212094534768</v>
+      </c>
+      <c r="H45" s="21">
         <v>11459</v>
       </c>
-      <c r="G45" s="21">
+      <c r="I45" s="21">
         <v>11459</v>
+      </c>
+      <c r="J45" s="21">
+        <v>11437</v>
       </c>
     </row>
     <row r="46" ht="14.25">
@@ -6635,22 +7331,33 @@
         <v>44</v>
       </c>
       <c r="C46" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H46</f>
         <v>3.6043616381900918</v>
       </c>
       <c r="D46" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I46</f>
         <v>3.6043616381900918</v>
       </c>
       <c r="E46" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J46</f>
+        <v>3.7562086832231554</v>
+      </c>
+      <c r="F46" s="20">
+        <f>ABS(C46-D46)</f>
         <v>0</v>
       </c>
-      <c r="F46" s="21">
+      <c r="G46" s="20">
+        <f>ABS(C46-E46)</f>
+        <v>0.15184704503306357</v>
+      </c>
+      <c r="H46" s="21">
         <v>11647</v>
       </c>
-      <c r="G46" s="21">
+      <c r="I46" s="21">
         <v>11647</v>
+      </c>
+      <c r="J46" s="21">
+        <v>11194</v>
       </c>
     </row>
     <row r="47" ht="14.25">
@@ -6658,22 +7365,33 @@
         <v>45</v>
       </c>
       <c r="C47" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H47</f>
         <v>3.6708639384400139</v>
       </c>
       <c r="D47" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I47</f>
         <v>3.6692596800978934</v>
       </c>
       <c r="E47" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J47</f>
+        <v>3.678652668416448</v>
+      </c>
+      <c r="F47" s="20">
+        <f>ABS(C47-D47)</f>
         <v>0.0016042583421205237</v>
       </c>
-      <c r="F47" s="21">
+      <c r="G47" s="20">
+        <f>ABS(C47-E47)</f>
+        <v>0.0077887299764340945</v>
+      </c>
+      <c r="H47" s="21">
         <v>11436</v>
       </c>
-      <c r="G47" s="21">
+      <c r="I47" s="21">
         <v>11441</v>
+      </c>
+      <c r="J47" s="21">
+        <v>11430</v>
       </c>
     </row>
     <row r="48" ht="14.25">
@@ -6681,22 +7399,33 @@
         <v>46</v>
       </c>
       <c r="C48" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H48</f>
         <v>3.6164713990351482</v>
       </c>
       <c r="D48" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I48</f>
         <v>3.6155369907846007</v>
       </c>
       <c r="E48" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J48</f>
+        <v>3.7521863287524542</v>
+      </c>
+      <c r="F48" s="20">
+        <f>ABS(C48-D48)</f>
         <v>0.00093440825054758037</v>
       </c>
-      <c r="F48" s="21">
+      <c r="G48" s="20">
+        <f>ABS(C48-E48)</f>
+        <v>0.13571492971730592</v>
+      </c>
+      <c r="H48" s="21">
         <v>11608</v>
       </c>
-      <c r="G48" s="21">
+      <c r="I48" s="21">
         <v>11611</v>
+      </c>
+      <c r="J48" s="21">
+        <v>11206</v>
       </c>
     </row>
     <row r="49" ht="14.25">
@@ -6704,22 +7433,33 @@
         <v>47</v>
       </c>
       <c r="C49" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H49</f>
         <v>3.676650902084428</v>
       </c>
       <c r="D49" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I49</f>
         <v>3.6702220667948944</v>
       </c>
       <c r="E49" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J49</f>
+        <v>3.6851007887817704</v>
+      </c>
+      <c r="F49" s="20">
+        <f>ABS(C49-D49)</f>
         <v>0.0064288352895336409</v>
       </c>
-      <c r="F49" s="21">
+      <c r="G49" s="20">
+        <f>ABS(C49-E49)</f>
+        <v>0.0084498866973423681</v>
+      </c>
+      <c r="H49" s="21">
         <v>11418</v>
       </c>
-      <c r="G49" s="21">
+      <c r="I49" s="21">
         <v>11438</v>
+      </c>
+      <c r="J49" s="21">
+        <v>11410</v>
       </c>
     </row>
     <row r="50" ht="14.25">
@@ -6727,22 +7467,33 @@
         <v>48</v>
       </c>
       <c r="C50" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H50</f>
         <v>3.6220880069025023</v>
       </c>
       <c r="D50" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I50</f>
         <v>3.6220880069025023</v>
       </c>
       <c r="E50" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J50</f>
+        <v>3.7582230961744725</v>
+      </c>
+      <c r="F50" s="20">
+        <f>ABS(C50-D50)</f>
         <v>0</v>
       </c>
-      <c r="F50" s="21">
+      <c r="G50" s="20">
+        <f>ABS(C50-E50)</f>
+        <v>0.13613508927197016</v>
+      </c>
+      <c r="H50" s="21">
         <v>11590</v>
       </c>
-      <c r="G50" s="21">
+      <c r="I50" s="21">
         <v>11590</v>
+      </c>
+      <c r="J50" s="21">
+        <v>11188</v>
       </c>
     </row>
     <row r="51" ht="14.25">
@@ -6750,22 +7501,33 @@
         <v>49</v>
       </c>
       <c r="C51" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H51</f>
         <v>3.6792287467134095</v>
       </c>
       <c r="D51" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I51</f>
         <v>3.6795512314839161</v>
       </c>
       <c r="E51" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J51</f>
+        <v>3.6909234550561796</v>
+      </c>
+      <c r="F51" s="20">
+        <f>ABS(C51-D51)</f>
         <v>0.00032248477050655922</v>
       </c>
-      <c r="F51" s="21">
+      <c r="G51" s="20">
+        <f>ABS(C51-E51)</f>
+        <v>0.011694708342770088</v>
+      </c>
+      <c r="H51" s="21">
         <v>11410</v>
       </c>
-      <c r="G51" s="21">
+      <c r="I51" s="21">
         <v>11409</v>
+      </c>
+      <c r="J51" s="21">
+        <v>11392</v>
       </c>
     </row>
     <row r="52" ht="14.25">
@@ -6773,22 +7535,33 @@
         <v>50</v>
       </c>
       <c r="C52" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H52</f>
         <v>3.6242769576102911</v>
       </c>
       <c r="D52" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I52</f>
         <v>3.625842114354811</v>
       </c>
       <c r="E52" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J52</f>
+        <v>3.7622584108804582</v>
+      </c>
+      <c r="F52" s="20">
+        <f>ABS(C52-D52)</f>
         <v>0.0015651567445198467</v>
       </c>
-      <c r="F52" s="21">
+      <c r="G52" s="20">
+        <f>ABS(C52-E52)</f>
+        <v>0.13798145327016709</v>
+      </c>
+      <c r="H52" s="21">
         <v>11583</v>
       </c>
-      <c r="G52" s="21">
+      <c r="I52" s="21">
         <v>11578</v>
+      </c>
+      <c r="J52" s="21">
+        <v>11176</v>
       </c>
     </row>
     <row r="53" ht="14.25">
@@ -6796,22 +7569,33 @@
         <v>51</v>
       </c>
       <c r="C53" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H53</f>
         <v>3.6843952957697033</v>
       </c>
       <c r="D53" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I53</f>
         <v>3.6840719613865729</v>
       </c>
       <c r="E53" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J53</f>
+        <v>3.6970895981711069</v>
+      </c>
+      <c r="F53" s="20">
+        <f>ABS(C53-D53)</f>
         <v>0.00032333438313036922</v>
       </c>
-      <c r="F53" s="21">
+      <c r="G53" s="20">
+        <f>ABS(C53-E53)</f>
+        <v>0.012694302401403679</v>
+      </c>
+      <c r="H53" s="21">
         <v>11394</v>
       </c>
-      <c r="G53" s="21">
+      <c r="I53" s="21">
         <v>11395</v>
+      </c>
+      <c r="J53" s="21">
+        <v>11373</v>
       </c>
     </row>
     <row r="54" ht="14.25">
@@ -6819,22 +7603,33 @@
         <v>52</v>
       </c>
       <c r="C54" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H54</f>
         <v>3.6327448944271374</v>
       </c>
       <c r="D54" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I54</f>
         <v>3.6324305615644197</v>
       </c>
       <c r="E54" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J54</f>
+        <v>3.7585590417448826</v>
+      </c>
+      <c r="F54" s="20">
+        <f>ABS(C54-D54)</f>
         <v>0.00031433286271775884</v>
       </c>
-      <c r="F54" s="21">
+      <c r="G54" s="20">
+        <f>ABS(C54-E54)</f>
+        <v>0.12581414731774521</v>
+      </c>
+      <c r="H54" s="21">
         <v>11556</v>
       </c>
-      <c r="G54" s="21">
+      <c r="I54" s="21">
         <v>11557</v>
+      </c>
+      <c r="J54" s="21">
+        <v>11187</v>
       </c>
     </row>
     <row r="55" ht="14.25">
@@ -6842,22 +7637,33 @@
         <v>53</v>
       </c>
       <c r="C55" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H55</f>
         <v>3.6899006768040783</v>
       </c>
       <c r="D55" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I55</f>
         <v>3.6905494505494505</v>
       </c>
       <c r="E55" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J55</f>
+        <v>3.706214191273689</v>
+      </c>
+      <c r="F55" s="20">
+        <f>ABS(C55-D55)</f>
         <v>0.00064877374537219978</v>
       </c>
-      <c r="F55" s="21">
+      <c r="G55" s="20">
+        <f>ABS(C55-E55)</f>
+        <v>0.016313514469610713</v>
+      </c>
+      <c r="H55" s="21">
         <v>11377</v>
       </c>
-      <c r="G55" s="21">
+      <c r="I55" s="21">
         <v>11375</v>
+      </c>
+      <c r="J55" s="21">
+        <v>11345</v>
       </c>
     </row>
     <row r="56" ht="14.25">
@@ -6865,22 +7671,33 @@
         <v>54</v>
       </c>
       <c r="C56" s="20">
-        <f t="shared" si="9"/>
+        <f>$H$3/H56</f>
         <v>3.6393584742089296</v>
       </c>
       <c r="D56" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I56</f>
         <v>3.6393584742089296</v>
       </c>
       <c r="E56" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J56</f>
+        <v>3.7548669405250936</v>
+      </c>
+      <c r="F56" s="20">
+        <f>ABS(C56-D56)</f>
         <v>0</v>
       </c>
-      <c r="F56" s="21">
+      <c r="G56" s="20">
+        <f>ABS(C56-E56)</f>
+        <v>0.11550846631616407</v>
+      </c>
+      <c r="H56" s="21">
         <v>11535</v>
       </c>
-      <c r="G56" s="21">
+      <c r="I56" s="21">
         <v>11535</v>
+      </c>
+      <c r="J56" s="21">
+        <v>11198</v>
       </c>
     </row>
     <row r="57" ht="14.25">
@@ -6888,22 +7705,33 @@
         <v>55</v>
       </c>
       <c r="C57" s="24">
-        <f t="shared" si="9"/>
+        <f>$H$3/H57</f>
         <v>3.6947720471747934</v>
       </c>
       <c r="D57" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I57</f>
         <v>3.6954225352112675</v>
       </c>
       <c r="E57" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J57</f>
+        <v>3.7045814977973568</v>
+      </c>
+      <c r="F57" s="20">
+        <f>ABS(C57-D57)</f>
         <v>0.00065048803647416165</v>
       </c>
-      <c r="F57" s="22">
+      <c r="G57" s="20">
+        <f>ABS(C57-E57)</f>
+        <v>0.0098094506225634426</v>
+      </c>
+      <c r="H57" s="22">
         <v>11362</v>
       </c>
-      <c r="G57" s="21">
+      <c r="I57" s="21">
         <v>11360</v>
+      </c>
+      <c r="J57" s="21">
+        <v>11350</v>
       </c>
     </row>
     <row r="58" ht="14.25">
@@ -6911,22 +7739,33 @@
         <v>56</v>
       </c>
       <c r="C58" s="24">
-        <f t="shared" si="9"/>
+        <f>$H$3/H58</f>
         <v>3.6459961785652251</v>
       </c>
       <c r="D58" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I58</f>
         <v>3.6472632493483927</v>
       </c>
       <c r="E58" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J58</f>
+        <v>3.7592311130978988</v>
+      </c>
+      <c r="F58" s="20">
+        <f>ABS(C58-D58)</f>
         <v>0.0012670707831676786</v>
       </c>
-      <c r="F58" s="22">
+      <c r="G58" s="20">
+        <f>ABS(C58-E58)</f>
+        <v>0.11323493453267375</v>
+      </c>
+      <c r="H58" s="22">
         <v>11514</v>
       </c>
-      <c r="G58" s="21">
+      <c r="I58" s="21">
         <v>11510</v>
+      </c>
+      <c r="J58" s="21">
+        <v>11185</v>
       </c>
     </row>
     <row r="59" ht="14.25">
@@ -6934,22 +7773,33 @@
         <v>57</v>
       </c>
       <c r="C59" s="24">
-        <f t="shared" si="9"/>
+        <f>$H$3/H59</f>
         <v>3.6977010481810977</v>
       </c>
       <c r="D59" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I59</f>
         <v>3.6963986968389539</v>
       </c>
       <c r="E59" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J59</f>
+        <v>3.7078483245149911</v>
+      </c>
+      <c r="F59" s="20">
+        <f>ABS(C59-D59)</f>
         <v>0.0013023513421437372</v>
       </c>
-      <c r="F59" s="22">
+      <c r="G59" s="20">
+        <f>ABS(C59-E59)</f>
+        <v>0.010147276333893451</v>
+      </c>
+      <c r="H59" s="22">
         <v>11353</v>
       </c>
-      <c r="G59" s="21">
+      <c r="I59" s="21">
         <v>11357</v>
+      </c>
+      <c r="J59" s="21">
+        <v>11340</v>
       </c>
     </row>
     <row r="60" ht="14.25">
@@ -6957,22 +7807,33 @@
         <v>58</v>
       </c>
       <c r="C60" s="24">
-        <f t="shared" si="9"/>
+        <f>$H$3/H60</f>
         <v>3.6501173810972958</v>
       </c>
       <c r="D60" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I60</f>
         <v>3.6485312011124629</v>
       </c>
       <c r="E60" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J60</f>
+        <v>3.7673147567422274</v>
+      </c>
+      <c r="F60" s="20">
+        <f>ABS(C60-D60)</f>
         <v>0.0015861799848329028</v>
       </c>
-      <c r="F60" s="22">
+      <c r="G60" s="20">
+        <f>ABS(C60-E60)</f>
+        <v>0.1171973756449316</v>
+      </c>
+      <c r="H60" s="22">
         <v>11501</v>
       </c>
-      <c r="G60" s="22">
+      <c r="I60" s="22">
         <v>11506</v>
+      </c>
+      <c r="J60" s="22">
+        <v>11161</v>
       </c>
     </row>
     <row r="61" ht="14.25">
@@ -6980,22 +7841,33 @@
         <v>59</v>
       </c>
       <c r="C61" s="24">
-        <f t="shared" si="9"/>
+        <f>$H$3/H61</f>
         <v>3.6986784140969164</v>
       </c>
       <c r="D61" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I61</f>
         <v>3.6983525680556779</v>
       </c>
       <c r="E61" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J61</f>
+        <v>3.7137431549196256</v>
+      </c>
+      <c r="F61" s="20">
+        <f>ABS(C61-D61)</f>
         <v>0.00032584604123853111</v>
       </c>
-      <c r="F61" s="22">
+      <c r="G61" s="20">
+        <f>ABS(C61-E61)</f>
+        <v>0.015064740822709144</v>
+      </c>
+      <c r="H61" s="22">
         <v>11350</v>
       </c>
-      <c r="G61" s="22">
+      <c r="I61" s="22">
         <v>11351</v>
+      </c>
+      <c r="J61" s="22">
+        <v>11322</v>
       </c>
     </row>
     <row r="62" ht="14.25">
@@ -7003,22 +7875,33 @@
         <v>60</v>
       </c>
       <c r="C62" s="24">
-        <f t="shared" si="9"/>
+        <f>$H$3/H62</f>
         <v>3.6529759832927255</v>
       </c>
       <c r="D62" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I62</f>
         <v>3.6520226185297955</v>
       </c>
       <c r="E62" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J62</f>
+        <v>3.7666397921705634</v>
+      </c>
+      <c r="F62" s="20">
+        <f>ABS(C62-D62)</f>
         <v>0.00095336476293006456</v>
       </c>
-      <c r="F62" s="22">
+      <c r="G62" s="20">
+        <f>ABS(C62-E62)</f>
+        <v>0.11366380887783789</v>
+      </c>
+      <c r="H62" s="22">
         <v>11492</v>
       </c>
-      <c r="G62" s="22">
+      <c r="I62" s="22">
         <v>11495</v>
+      </c>
+      <c r="J62" s="22">
+        <v>11163</v>
       </c>
     </row>
     <row r="63" ht="14.25">
@@ -7026,22 +7909,33 @@
         <v>61</v>
       </c>
       <c r="C63" s="24">
-        <f t="shared" si="9"/>
+        <f>$H$3/H63</f>
         <v>3.6980267794221282</v>
       </c>
       <c r="D63" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I63</f>
         <v>3.7009609450762584</v>
       </c>
       <c r="E63" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J63</f>
+        <v>3.7147274494213272</v>
+      </c>
+      <c r="F63" s="20">
+        <f>ABS(C63-D63)</f>
         <v>0.002934165654130183</v>
       </c>
-      <c r="F63" s="22">
+      <c r="G63" s="20">
+        <f>ABS(C63-E63)</f>
+        <v>0.016700669999198947</v>
+      </c>
+      <c r="H63" s="22">
         <v>11352</v>
       </c>
-      <c r="G63" s="22">
+      <c r="I63" s="22">
         <v>11343</v>
+      </c>
+      <c r="J63" s="22">
+        <v>11319</v>
       </c>
     </row>
     <row r="64" ht="14.25">
@@ -7049,22 +7943,33 @@
         <v>62</v>
       </c>
       <c r="C64" s="24">
-        <f t="shared" si="9"/>
+        <f>$H$3/H64</f>
         <v>3.6571129889363183</v>
       </c>
       <c r="D64" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I64</f>
         <v>3.6548842068605261</v>
       </c>
       <c r="E64" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J64</f>
+        <v>3.7622584108804582</v>
+      </c>
+      <c r="F64" s="20">
+        <f>ABS(C64-D64)</f>
         <v>0.0022287820757922461</v>
       </c>
-      <c r="F64" s="22">
+      <c r="G64" s="20">
+        <f>ABS(C64-E64)</f>
+        <v>0.10514542194413989</v>
+      </c>
+      <c r="H64" s="22">
         <v>11479</v>
       </c>
-      <c r="G64" s="22">
+      <c r="I64" s="22">
         <v>11486</v>
+      </c>
+      <c r="J64" s="22">
+        <v>11176</v>
       </c>
     </row>
     <row r="65" ht="14.25">
@@ -7072,22 +7977,33 @@
         <v>63</v>
       </c>
       <c r="C65" s="24">
-        <f t="shared" si="9"/>
+        <f>$H$3/H65</f>
         <v>3.7003085059497578</v>
       </c>
       <c r="D65" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I65</f>
         <v>3.6999823726423409</v>
       </c>
       <c r="E65" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J65</f>
+        <v>3.7180122026704394</v>
+      </c>
+      <c r="F65" s="20">
+        <f>ABS(C65-D65)</f>
         <v>0.00032613330741693147</v>
       </c>
-      <c r="F65" s="22">
+      <c r="G65" s="20">
+        <f>ABS(C65-E65)</f>
+        <v>0.017703696720681616</v>
+      </c>
+      <c r="H65" s="22">
         <v>11345</v>
       </c>
-      <c r="G65" s="22">
+      <c r="I65" s="22">
         <v>11346</v>
+      </c>
+      <c r="J65" s="22">
+        <v>11309</v>
       </c>
     </row>
     <row r="66" ht="14.25">
@@ -7095,22 +8011,33 @@
         <v>64</v>
       </c>
       <c r="C66" s="24">
-        <f t="shared" si="9"/>
+        <f>$H$3/H66</f>
         <v>3.6599825632083696</v>
       </c>
       <c r="D66" s="20">
-        <f t="shared" si="10"/>
+        <f>$I$3/I66</f>
         <v>3.6590255382201691</v>
       </c>
       <c r="E66" s="20">
-        <f t="shared" si="11"/>
+        <f>$J$3/J66</f>
+        <v>3.767652329749104</v>
+      </c>
+      <c r="F66" s="20">
+        <f>ABS(C66-D66)</f>
         <v>0.00095702498820049442</v>
       </c>
-      <c r="F66" s="22">
+      <c r="G66" s="20">
+        <f>ABS(C66-E66)</f>
+        <v>0.10766976654073446</v>
+      </c>
+      <c r="H66" s="22">
         <v>11470</v>
       </c>
-      <c r="G66" s="22">
+      <c r="I66" s="22">
         <v>11473</v>
+      </c>
+      <c r="J66" s="22">
+        <v>11160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>